<commit_message>
added occurrence and items for Yellow Warbler
</commit_message>
<xml_diff>
--- a/AvianDietDatabase_King_1883_AD.xlsx
+++ b/AvianDietDatabase_King_1883_AD.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="AvianDietDatabase_King_1883" localSheetId="0">Sheet1!$A$1:$AO$107</definedName>
+    <definedName name="AvianDietDatabase_King_1883" localSheetId="0">Sheet1!$A$1:$AO$111</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="155">
   <si>
     <t>Common_Name</t>
   </si>
@@ -491,6 +491,21 @@
   </si>
   <si>
     <t>plant lice</t>
+  </si>
+  <si>
+    <t>Blue-eyed Yellow Warbler</t>
+  </si>
+  <si>
+    <t>Dendroica aestiva</t>
+  </si>
+  <si>
+    <t>insect larvae</t>
+  </si>
+  <si>
+    <t>urban; woodland</t>
+  </si>
+  <si>
+    <t>AHD</t>
   </si>
 </sst>
 </file>
@@ -812,11 +827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO107"/>
+  <dimension ref="A1:AO111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE98" sqref="AE98"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM64" sqref="AM64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,7 +2700,7 @@
         <v>57</v>
       </c>
       <c r="AN17" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO17" t="s">
         <v>59</v>
@@ -2789,7 +2804,7 @@
         <v>57</v>
       </c>
       <c r="AN18" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO18" t="s">
         <v>59</v>
@@ -2896,7 +2911,7 @@
         <v>57</v>
       </c>
       <c r="AN19" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO19" t="s">
         <v>59</v>
@@ -3000,7 +3015,7 @@
         <v>57</v>
       </c>
       <c r="AN20" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO20" t="s">
         <v>59</v>
@@ -3110,7 +3125,7 @@
         <v>57</v>
       </c>
       <c r="AN21" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO21" t="s">
         <v>59</v>
@@ -3220,7 +3235,7 @@
         <v>57</v>
       </c>
       <c r="AN22" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO22" t="s">
         <v>59</v>
@@ -3327,7 +3342,7 @@
         <v>57</v>
       </c>
       <c r="AN23" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO23" t="s">
         <v>59</v>
@@ -3437,7 +3452,7 @@
         <v>57</v>
       </c>
       <c r="AN24" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO24" t="s">
         <v>59</v>
@@ -6976,10 +6991,10 @@
     </row>
     <row r="58" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
         <v>43</v>
@@ -7009,22 +7024,22 @@
         <v>46</v>
       </c>
       <c r="L58" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M58" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="N58">
         <v>7</v>
       </c>
       <c r="O58">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P58">
         <v>7</v>
       </c>
       <c r="Q58">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R58" t="s">
         <v>49</v>
@@ -7053,17 +7068,20 @@
       <c r="AE58" t="s">
         <v>43</v>
       </c>
+      <c r="AF58" t="s">
+        <v>147</v>
+      </c>
       <c r="AG58">
-        <v>0.45454549999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AH58" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI58" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI58">
+        <v>4</v>
       </c>
       <c r="AJ58">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AK58">
         <v>1</v>
@@ -7072,7 +7090,7 @@
         <v>57</v>
       </c>
       <c r="AN58" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO58" t="s">
         <v>59</v>
@@ -7080,10 +7098,10 @@
     </row>
     <row r="59" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
         <v>43</v>
@@ -7113,22 +7131,22 @@
         <v>46</v>
       </c>
       <c r="L59" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M59" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="N59">
         <v>7</v>
       </c>
       <c r="O59">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P59">
         <v>7</v>
       </c>
       <c r="Q59">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R59" t="s">
         <v>49</v>
@@ -7142,41 +7160,35 @@
       <c r="U59" t="s">
         <v>52</v>
       </c>
-      <c r="V59" t="s">
-        <v>60</v>
-      </c>
-      <c r="W59" t="s">
-        <v>105</v>
-      </c>
-      <c r="X59" t="s">
-        <v>106</v>
-      </c>
       <c r="AA59" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB59">
-        <v>118840</v>
+        <v>99208</v>
       </c>
       <c r="AC59" t="s">
         <v>55</v>
       </c>
+      <c r="AD59" t="s">
+        <v>65</v>
+      </c>
       <c r="AE59" t="s">
         <v>43</v>
       </c>
       <c r="AF59" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="AG59">
-        <v>9.0909089999999998E-2</v>
+        <v>0.5</v>
       </c>
       <c r="AH59" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI59" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI59">
+        <v>4</v>
       </c>
       <c r="AJ59">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AK59">
         <v>1</v>
@@ -7185,7 +7197,7 @@
         <v>57</v>
       </c>
       <c r="AN59" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO59" t="s">
         <v>59</v>
@@ -7193,10 +7205,10 @@
     </row>
     <row r="60" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C60" t="s">
         <v>43</v>
@@ -7226,22 +7238,22 @@
         <v>46</v>
       </c>
       <c r="L60" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M60" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="N60">
         <v>7</v>
       </c>
       <c r="O60">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P60">
         <v>7</v>
       </c>
       <c r="Q60">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R60" t="s">
         <v>49</v>
@@ -7256,16 +7268,13 @@
         <v>52</v>
       </c>
       <c r="V60" t="s">
-        <v>61</v>
-      </c>
-      <c r="W60" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="AA60" t="s">
         <v>54</v>
       </c>
       <c r="AB60">
-        <v>109185</v>
+        <v>109216</v>
       </c>
       <c r="AC60" t="s">
         <v>55</v>
@@ -7273,8 +7282,11 @@
       <c r="AE60" t="s">
         <v>43</v>
       </c>
+      <c r="AF60" t="s">
+        <v>147</v>
+      </c>
       <c r="AG60">
-        <v>9.0909089999999998E-2</v>
+        <v>0.4</v>
       </c>
       <c r="AH60" t="s">
         <v>56</v>
@@ -7283,7 +7295,7 @@
         <v>43</v>
       </c>
       <c r="AJ60">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AK60">
         <v>1</v>
@@ -7292,7 +7304,7 @@
         <v>57</v>
       </c>
       <c r="AN60" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO60" t="s">
         <v>59</v>
@@ -7300,10 +7312,10 @@
     </row>
     <row r="61" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C61" t="s">
         <v>43</v>
@@ -7333,22 +7345,22 @@
         <v>46</v>
       </c>
       <c r="L61" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M61" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="N61">
         <v>7</v>
       </c>
       <c r="O61">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P61">
         <v>7</v>
       </c>
       <c r="Q61">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R61" t="s">
         <v>49</v>
@@ -7362,23 +7374,26 @@
       <c r="U61" t="s">
         <v>52</v>
       </c>
-      <c r="V61" t="s">
-        <v>63</v>
-      </c>
       <c r="AA61" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB61">
-        <v>152741</v>
+        <v>99208</v>
       </c>
       <c r="AC61" t="s">
         <v>55</v>
       </c>
+      <c r="AD61" t="s">
+        <v>65</v>
+      </c>
       <c r="AE61" t="s">
         <v>43</v>
       </c>
+      <c r="AF61" t="s">
+        <v>152</v>
+      </c>
       <c r="AG61">
-        <v>9.0909089999999998E-2</v>
+        <v>0.4</v>
       </c>
       <c r="AH61" t="s">
         <v>56</v>
@@ -7387,7 +7402,7 @@
         <v>43</v>
       </c>
       <c r="AJ61">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AK61">
         <v>1</v>
@@ -7396,13 +7411,13 @@
         <v>57</v>
       </c>
       <c r="AN61" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>111</v>
       </c>
@@ -7467,25 +7482,22 @@
         <v>52</v>
       </c>
       <c r="V62" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AA62" t="s">
         <v>54</v>
       </c>
       <c r="AB62">
-        <v>117232</v>
+        <v>109216</v>
       </c>
       <c r="AC62" t="s">
         <v>55</v>
       </c>
-      <c r="AD62" t="s">
-        <v>65</v>
-      </c>
       <c r="AE62" t="s">
         <v>43</v>
       </c>
       <c r="AG62">
-        <v>0.18181820000000001</v>
+        <v>0.45454549999999999</v>
       </c>
       <c r="AH62" t="s">
         <v>56</v>
@@ -7501,9 +7513,6 @@
       </c>
       <c r="AL62" t="s">
         <v>57</v>
-      </c>
-      <c r="AM62" t="s">
-        <v>99</v>
       </c>
       <c r="AN62" t="s">
         <v>58</v>
@@ -7577,19 +7586,28 @@
         <v>52</v>
       </c>
       <c r="V63" t="s">
-        <v>117</v>
+        <v>60</v>
+      </c>
+      <c r="W63" t="s">
+        <v>105</v>
+      </c>
+      <c r="X63" t="s">
+        <v>106</v>
       </c>
       <c r="AA63" t="s">
         <v>54</v>
       </c>
       <c r="AB63">
-        <v>102160</v>
+        <v>118840</v>
       </c>
       <c r="AC63" t="s">
         <v>55</v>
       </c>
       <c r="AE63" t="s">
         <v>43</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>115</v>
       </c>
       <c r="AG63">
         <v>9.0909089999999998E-2</v>
@@ -7681,13 +7699,16 @@
         <v>52</v>
       </c>
       <c r="V64" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="W64" t="s">
+        <v>116</v>
       </c>
       <c r="AA64" t="s">
         <v>54</v>
       </c>
       <c r="AB64">
-        <v>152741</v>
+        <v>109185</v>
       </c>
       <c r="AC64" t="s">
         <v>55</v>
@@ -7695,17 +7716,14 @@
       <c r="AE64" t="s">
         <v>43</v>
       </c>
-      <c r="AF64" t="s">
-        <v>146</v>
-      </c>
       <c r="AG64">
-        <v>8.3333333333333329E-2</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH64" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI64">
-        <v>36</v>
+        <v>56</v>
+      </c>
+      <c r="AI64" t="s">
+        <v>43</v>
       </c>
       <c r="AJ64">
         <v>11</v>
@@ -7788,34 +7806,28 @@
         <v>52</v>
       </c>
       <c r="V65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA65" t="s">
         <v>54</v>
       </c>
       <c r="AB65">
-        <v>117232</v>
+        <v>152741</v>
       </c>
       <c r="AC65" t="s">
         <v>55</v>
       </c>
-      <c r="AD65" t="s">
-        <v>65</v>
-      </c>
       <c r="AE65" t="s">
         <v>43</v>
       </c>
-      <c r="AF65" t="s">
-        <v>73</v>
-      </c>
       <c r="AG65">
-        <v>0.1111111111111111</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH65" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI65">
-        <v>36</v>
+        <v>56</v>
+      </c>
+      <c r="AI65" t="s">
+        <v>43</v>
       </c>
       <c r="AJ65">
         <v>11</v>
@@ -7898,37 +7910,31 @@
         <v>52</v>
       </c>
       <c r="V66" t="s">
-        <v>60</v>
-      </c>
-      <c r="W66" t="s">
-        <v>105</v>
-      </c>
-      <c r="X66" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="AA66" t="s">
         <v>54</v>
       </c>
       <c r="AB66">
-        <v>118840</v>
+        <v>117232</v>
       </c>
       <c r="AC66" t="s">
         <v>55</v>
       </c>
+      <c r="AD66" t="s">
+        <v>65</v>
+      </c>
       <c r="AE66" t="s">
         <v>43</v>
       </c>
-      <c r="AF66" t="s">
-        <v>115</v>
-      </c>
       <c r="AG66">
-        <v>2.7777777777777776E-2</v>
+        <v>0.18181820000000001</v>
       </c>
       <c r="AH66" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI66">
-        <v>36</v>
+        <v>56</v>
+      </c>
+      <c r="AI66" t="s">
+        <v>43</v>
       </c>
       <c r="AJ66">
         <v>11</v>
@@ -7938,6 +7944,9 @@
       </c>
       <c r="AL66" t="s">
         <v>57</v>
+      </c>
+      <c r="AM66" t="s">
+        <v>99</v>
       </c>
       <c r="AN66" t="s">
         <v>58</v>
@@ -8011,13 +8020,13 @@
         <v>52</v>
       </c>
       <c r="V67" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="AA67" t="s">
         <v>54</v>
       </c>
       <c r="AB67">
-        <v>109216</v>
+        <v>102160</v>
       </c>
       <c r="AC67" t="s">
         <v>55</v>
@@ -8025,17 +8034,14 @@
       <c r="AE67" t="s">
         <v>43</v>
       </c>
-      <c r="AF67" t="s">
-        <v>147</v>
-      </c>
       <c r="AG67">
-        <v>0.33333333333333331</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH67" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI67">
-        <v>36</v>
+        <v>56</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>43</v>
       </c>
       <c r="AJ67">
         <v>11</v>
@@ -8118,16 +8124,13 @@
         <v>52</v>
       </c>
       <c r="V68" t="s">
-        <v>61</v>
-      </c>
-      <c r="W68" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="AA68" t="s">
         <v>54</v>
       </c>
       <c r="AB68">
-        <v>109185</v>
+        <v>152741</v>
       </c>
       <c r="AC68" t="s">
         <v>55</v>
@@ -8136,10 +8139,10 @@
         <v>43</v>
       </c>
       <c r="AF68" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AG68">
-        <v>0.41666666666666669</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AH68" t="s">
         <v>90</v>
@@ -8157,7 +8160,7 @@
         <v>57</v>
       </c>
       <c r="AN68" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO68" t="s">
         <v>59</v>
@@ -8228,25 +8231,28 @@
         <v>52</v>
       </c>
       <c r="V69" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="AA69" t="s">
         <v>54</v>
       </c>
       <c r="AB69">
-        <v>102160</v>
+        <v>117232</v>
       </c>
       <c r="AC69" t="s">
         <v>55</v>
       </c>
+      <c r="AD69" t="s">
+        <v>65</v>
+      </c>
       <c r="AE69" t="s">
         <v>43</v>
       </c>
       <c r="AF69" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="AG69">
-        <v>2.7777777777777776E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="AH69" t="s">
         <v>90</v>
@@ -8264,7 +8270,7 @@
         <v>57</v>
       </c>
       <c r="AN69" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO69" t="s">
         <v>59</v>
@@ -8272,10 +8278,10 @@
     </row>
     <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C70" t="s">
         <v>43</v>
@@ -8305,22 +8311,22 @@
         <v>46</v>
       </c>
       <c r="L70" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="M70" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="N70">
         <v>7</v>
       </c>
       <c r="O70">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="P70">
         <v>7</v>
       </c>
       <c r="Q70">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="R70" t="s">
         <v>49</v>
@@ -8335,13 +8341,19 @@
         <v>52</v>
       </c>
       <c r="V70" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="W70" t="s">
+        <v>105</v>
+      </c>
+      <c r="X70" t="s">
+        <v>106</v>
       </c>
       <c r="AA70" t="s">
         <v>54</v>
       </c>
       <c r="AB70">
-        <v>109216</v>
+        <v>118840</v>
       </c>
       <c r="AC70" t="s">
         <v>55</v>
@@ -8349,17 +8361,20 @@
       <c r="AE70" t="s">
         <v>43</v>
       </c>
+      <c r="AF70" t="s">
+        <v>115</v>
+      </c>
       <c r="AG70">
-        <v>0.35294120000000001</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="AH70" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI70" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI70">
+        <v>36</v>
       </c>
       <c r="AJ70">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="AK70">
         <v>1</v>
@@ -8368,7 +8383,7 @@
         <v>57</v>
       </c>
       <c r="AN70" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO70" t="s">
         <v>59</v>
@@ -8376,10 +8391,10 @@
     </row>
     <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
         <v>43</v>
@@ -8409,22 +8424,22 @@
         <v>46</v>
       </c>
       <c r="L71" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="M71" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="N71">
         <v>7</v>
       </c>
       <c r="O71">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="P71">
         <v>7</v>
       </c>
       <c r="Q71">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="R71" t="s">
         <v>49</v>
@@ -8439,13 +8454,13 @@
         <v>52</v>
       </c>
       <c r="V71" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="AA71" t="s">
         <v>54</v>
       </c>
       <c r="AB71">
-        <v>118831</v>
+        <v>109216</v>
       </c>
       <c r="AC71" t="s">
         <v>55</v>
@@ -8453,17 +8468,20 @@
       <c r="AE71" t="s">
         <v>43</v>
       </c>
+      <c r="AF71" t="s">
+        <v>147</v>
+      </c>
       <c r="AG71">
-        <v>0.35294120000000001</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AH71" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI71" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI71">
+        <v>36</v>
       </c>
       <c r="AJ71">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="AK71">
         <v>1</v>
@@ -8472,7 +8490,7 @@
         <v>57</v>
       </c>
       <c r="AN71" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO71" t="s">
         <v>59</v>
@@ -8480,10 +8498,10 @@
     </row>
     <row r="72" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B72" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
         <v>43</v>
@@ -8513,22 +8531,22 @@
         <v>46</v>
       </c>
       <c r="L72" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="M72" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="N72">
         <v>7</v>
       </c>
       <c r="O72">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="P72">
         <v>7</v>
       </c>
       <c r="Q72">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="R72" t="s">
         <v>49</v>
@@ -8543,13 +8561,16 @@
         <v>52</v>
       </c>
       <c r="V72" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="W72" t="s">
+        <v>116</v>
       </c>
       <c r="AA72" t="s">
         <v>54</v>
       </c>
       <c r="AB72">
-        <v>152741</v>
+        <v>109185</v>
       </c>
       <c r="AC72" t="s">
         <v>55</v>
@@ -8557,17 +8578,20 @@
       <c r="AE72" t="s">
         <v>43</v>
       </c>
+      <c r="AF72" t="s">
+        <v>149</v>
+      </c>
       <c r="AG72">
-        <v>0.23529410000000001</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="AH72" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI72" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI72">
+        <v>36</v>
       </c>
       <c r="AJ72">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="AK72">
         <v>1</v>
@@ -8576,7 +8600,7 @@
         <v>57</v>
       </c>
       <c r="AN72" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO72" t="s">
         <v>59</v>
@@ -8584,10 +8608,10 @@
     </row>
     <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C73" t="s">
         <v>43</v>
@@ -8617,22 +8641,22 @@
         <v>46</v>
       </c>
       <c r="L73" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="M73" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="N73">
         <v>7</v>
       </c>
       <c r="O73">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="P73">
         <v>7</v>
       </c>
       <c r="Q73">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="R73" t="s">
         <v>49</v>
@@ -8647,37 +8671,34 @@
         <v>52</v>
       </c>
       <c r="V73" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="AA73" t="s">
         <v>54</v>
       </c>
       <c r="AB73">
-        <v>117232</v>
+        <v>102160</v>
       </c>
       <c r="AC73" t="s">
         <v>55</v>
       </c>
-      <c r="AD73" t="s">
-        <v>65</v>
-      </c>
       <c r="AE73" t="s">
         <v>43</v>
       </c>
       <c r="AF73" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="AG73">
-        <v>5.8823529999999999E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="AH73" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI73" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI73">
+        <v>36</v>
       </c>
       <c r="AJ73">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="AK73">
         <v>1</v>
@@ -8686,7 +8707,7 @@
         <v>57</v>
       </c>
       <c r="AN73" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO73" t="s">
         <v>59</v>
@@ -8757,25 +8778,19 @@
         <v>52</v>
       </c>
       <c r="V74" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AA74" t="s">
         <v>54</v>
       </c>
       <c r="AB74">
-        <v>117232</v>
+        <v>109216</v>
       </c>
       <c r="AC74" t="s">
         <v>55</v>
       </c>
-      <c r="AD74" t="s">
-        <v>67</v>
-      </c>
       <c r="AE74" t="s">
         <v>43</v>
-      </c>
-      <c r="AF74" t="s">
-        <v>68</v>
       </c>
       <c r="AG74">
         <v>0.35294120000000001</v>
@@ -8804,10 +8819,10 @@
     </row>
     <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C75" t="s">
         <v>43</v>
@@ -8837,22 +8852,22 @@
         <v>46</v>
       </c>
       <c r="L75" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M75" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="N75">
         <v>7</v>
       </c>
       <c r="O75">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P75">
         <v>7</v>
       </c>
       <c r="Q75">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R75" t="s">
         <v>49</v>
@@ -8867,28 +8882,22 @@
         <v>52</v>
       </c>
       <c r="V75" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AA75" t="s">
         <v>54</v>
       </c>
       <c r="AB75">
-        <v>117232</v>
+        <v>118831</v>
       </c>
       <c r="AC75" t="s">
         <v>55</v>
       </c>
-      <c r="AD75" t="s">
-        <v>65</v>
-      </c>
       <c r="AE75" t="s">
         <v>43</v>
       </c>
-      <c r="AF75" t="s">
-        <v>73</v>
-      </c>
       <c r="AG75">
-        <v>1</v>
+        <v>0.35294120000000001</v>
       </c>
       <c r="AH75" t="s">
         <v>56</v>
@@ -8897,7 +8906,7 @@
         <v>43</v>
       </c>
       <c r="AJ75">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="AK75">
         <v>1</v>
@@ -8914,10 +8923,10 @@
     </row>
     <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C76" t="s">
         <v>43</v>
@@ -8947,22 +8956,22 @@
         <v>46</v>
       </c>
       <c r="L76" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M76" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="N76">
         <v>7</v>
       </c>
       <c r="O76">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P76">
         <v>7</v>
       </c>
       <c r="Q76">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R76" t="s">
         <v>49</v>
@@ -8976,11 +8985,14 @@
       <c r="U76" t="s">
         <v>52</v>
       </c>
+      <c r="V76" t="s">
+        <v>63</v>
+      </c>
       <c r="AA76" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB76">
-        <v>99208</v>
+        <v>152741</v>
       </c>
       <c r="AC76" t="s">
         <v>55</v>
@@ -8988,11 +9000,8 @@
       <c r="AE76" t="s">
         <v>43</v>
       </c>
-      <c r="AF76" t="s">
-        <v>122</v>
-      </c>
       <c r="AG76">
-        <v>1</v>
+        <v>0.23529410000000001</v>
       </c>
       <c r="AH76" t="s">
         <v>56</v>
@@ -9001,7 +9010,7 @@
         <v>43</v>
       </c>
       <c r="AJ76">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="AK76">
         <v>1</v>
@@ -9018,10 +9027,10 @@
     </row>
     <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B77" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C77" t="s">
         <v>43</v>
@@ -9060,13 +9069,13 @@
         <v>7</v>
       </c>
       <c r="O77">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P77">
         <v>7</v>
       </c>
       <c r="Q77">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R77" t="s">
         <v>49</v>
@@ -9081,22 +9090,28 @@
         <v>52</v>
       </c>
       <c r="V77" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="AA77" t="s">
         <v>54</v>
       </c>
       <c r="AB77">
-        <v>109216</v>
+        <v>117232</v>
       </c>
       <c r="AC77" t="s">
         <v>55</v>
       </c>
+      <c r="AD77" t="s">
+        <v>65</v>
+      </c>
       <c r="AE77" t="s">
         <v>43</v>
       </c>
+      <c r="AF77" t="s">
+        <v>66</v>
+      </c>
       <c r="AG77">
-        <v>0.25</v>
+        <v>5.8823529999999999E-2</v>
       </c>
       <c r="AH77" t="s">
         <v>56</v>
@@ -9105,7 +9120,7 @@
         <v>43</v>
       </c>
       <c r="AJ77">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AK77">
         <v>1</v>
@@ -9122,10 +9137,10 @@
     </row>
     <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C78" t="s">
         <v>43</v>
@@ -9164,13 +9179,13 @@
         <v>7</v>
       </c>
       <c r="O78">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P78">
         <v>7</v>
       </c>
       <c r="Q78">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R78" t="s">
         <v>49</v>
@@ -9185,22 +9200,28 @@
         <v>52</v>
       </c>
       <c r="V78" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AA78" t="s">
         <v>54</v>
       </c>
       <c r="AB78">
-        <v>118831</v>
+        <v>117232</v>
       </c>
       <c r="AC78" t="s">
         <v>55</v>
       </c>
+      <c r="AD78" t="s">
+        <v>67</v>
+      </c>
       <c r="AE78" t="s">
         <v>43</v>
       </c>
+      <c r="AF78" t="s">
+        <v>68</v>
+      </c>
       <c r="AG78">
-        <v>0.125</v>
+        <v>0.35294120000000001</v>
       </c>
       <c r="AH78" t="s">
         <v>56</v>
@@ -9209,7 +9230,7 @@
         <v>43</v>
       </c>
       <c r="AJ78">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AK78">
         <v>1</v>
@@ -9226,10 +9247,10 @@
     </row>
     <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B79" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C79" t="s">
         <v>43</v>
@@ -9259,22 +9280,22 @@
         <v>46</v>
       </c>
       <c r="L79" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="M79" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="N79">
         <v>7</v>
       </c>
       <c r="O79">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="P79">
         <v>7</v>
       </c>
       <c r="Q79">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="R79" t="s">
         <v>49</v>
@@ -9289,25 +9310,28 @@
         <v>52</v>
       </c>
       <c r="V79" t="s">
-        <v>61</v>
-      </c>
-      <c r="W79" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AA79" t="s">
         <v>54</v>
       </c>
       <c r="AB79">
-        <v>103358</v>
+        <v>117232</v>
       </c>
       <c r="AC79" t="s">
         <v>55</v>
       </c>
+      <c r="AD79" t="s">
+        <v>65</v>
+      </c>
       <c r="AE79" t="s">
         <v>43</v>
       </c>
+      <c r="AF79" t="s">
+        <v>73</v>
+      </c>
       <c r="AG79">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="AH79" t="s">
         <v>56</v>
@@ -9316,7 +9340,7 @@
         <v>43</v>
       </c>
       <c r="AJ79">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK79">
         <v>1</v>
@@ -9333,10 +9357,10 @@
     </row>
     <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C80" t="s">
         <v>43</v>
@@ -9366,22 +9390,22 @@
         <v>46</v>
       </c>
       <c r="L80" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="M80" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="N80">
         <v>7</v>
       </c>
       <c r="O80">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="P80">
         <v>7</v>
       </c>
       <c r="Q80">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="R80" t="s">
         <v>49</v>
@@ -9395,14 +9419,11 @@
       <c r="U80" t="s">
         <v>52</v>
       </c>
-      <c r="V80" t="s">
-        <v>63</v>
-      </c>
       <c r="AA80" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB80">
-        <v>152741</v>
+        <v>99208</v>
       </c>
       <c r="AC80" t="s">
         <v>55</v>
@@ -9410,8 +9431,11 @@
       <c r="AE80" t="s">
         <v>43</v>
       </c>
+      <c r="AF80" t="s">
+        <v>122</v>
+      </c>
       <c r="AG80">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="AH80" t="s">
         <v>56</v>
@@ -9420,7 +9444,7 @@
         <v>43</v>
       </c>
       <c r="AJ80">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK80">
         <v>1</v>
@@ -9500,25 +9524,22 @@
         <v>52</v>
       </c>
       <c r="V81" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AA81" t="s">
         <v>54</v>
       </c>
       <c r="AB81">
-        <v>117232</v>
+        <v>109216</v>
       </c>
       <c r="AC81" t="s">
         <v>55</v>
       </c>
-      <c r="AD81" t="s">
-        <v>65</v>
-      </c>
       <c r="AE81" t="s">
         <v>43</v>
       </c>
       <c r="AG81">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="AH81" t="s">
         <v>56</v>
@@ -9534,9 +9555,6 @@
       </c>
       <c r="AL81" t="s">
         <v>57</v>
-      </c>
-      <c r="AM81" t="s">
-        <v>99</v>
       </c>
       <c r="AN81" t="s">
         <v>58</v>
@@ -9547,10 +9565,10 @@
     </row>
     <row r="82" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C82" t="s">
         <v>43</v>
@@ -9580,25 +9598,25 @@
         <v>46</v>
       </c>
       <c r="L82" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="M82" t="s">
         <v>89</v>
       </c>
       <c r="N82">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O82">
         <v>1875</v>
       </c>
       <c r="P82">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q82">
         <v>1875</v>
       </c>
       <c r="R82" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="S82" t="s">
         <v>50</v>
@@ -9610,13 +9628,13 @@
         <v>52</v>
       </c>
       <c r="V82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA82" t="s">
         <v>54</v>
       </c>
       <c r="AB82">
-        <v>103359</v>
+        <v>118831</v>
       </c>
       <c r="AC82" t="s">
         <v>55</v>
@@ -9625,7 +9643,7 @@
         <v>43</v>
       </c>
       <c r="AG82">
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="AH82" t="s">
         <v>56</v>
@@ -9634,7 +9652,7 @@
         <v>43</v>
       </c>
       <c r="AJ82">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK82">
         <v>1</v>
@@ -9651,10 +9669,10 @@
     </row>
     <row r="83" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B83" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
         <v>43</v>
@@ -9684,34 +9702,46 @@
         <v>46</v>
       </c>
       <c r="L83" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="M83" t="s">
         <v>89</v>
       </c>
       <c r="N83">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O83">
         <v>1875</v>
       </c>
       <c r="P83">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q83">
         <v>1875</v>
       </c>
       <c r="R83" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="S83" t="s">
-        <v>128</v>
+        <v>50</v>
+      </c>
+      <c r="T83" t="s">
+        <v>51</v>
+      </c>
+      <c r="U83" t="s">
+        <v>52</v>
+      </c>
+      <c r="V83" t="s">
+        <v>61</v>
+      </c>
+      <c r="W83" t="s">
+        <v>62</v>
       </c>
       <c r="AA83" t="s">
         <v>54</v>
       </c>
       <c r="AB83">
-        <v>202422</v>
+        <v>103358</v>
       </c>
       <c r="AC83" t="s">
         <v>55</v>
@@ -9719,11 +9749,8 @@
       <c r="AE83" t="s">
         <v>43</v>
       </c>
-      <c r="AF83" t="s">
-        <v>129</v>
-      </c>
       <c r="AG83">
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="AH83" t="s">
         <v>56</v>
@@ -9732,7 +9759,7 @@
         <v>43</v>
       </c>
       <c r="AJ83">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK83">
         <v>1</v>
@@ -9749,10 +9776,10 @@
     </row>
     <row r="84" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C84" t="s">
         <v>43</v>
@@ -9785,19 +9812,19 @@
         <v>47</v>
       </c>
       <c r="M84" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N84">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O84">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P84">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q84">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R84" t="s">
         <v>49</v>
@@ -9812,22 +9839,22 @@
         <v>52</v>
       </c>
       <c r="V84" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="AA84" t="s">
         <v>54</v>
       </c>
       <c r="AB84">
-        <v>109216</v>
+        <v>152741</v>
       </c>
       <c r="AC84" t="s">
         <v>55</v>
       </c>
       <c r="AE84" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="AG84">
-        <v>0.18181820000000001</v>
+        <v>0.125</v>
       </c>
       <c r="AH84" t="s">
         <v>56</v>
@@ -9836,7 +9863,7 @@
         <v>43</v>
       </c>
       <c r="AJ84">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="AK84">
         <v>1</v>
@@ -9853,10 +9880,10 @@
     </row>
     <row r="85" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B85" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C85" t="s">
         <v>43</v>
@@ -9889,19 +9916,19 @@
         <v>47</v>
       </c>
       <c r="M85" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N85">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O85">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P85">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q85">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R85" t="s">
         <v>49</v>
@@ -9916,22 +9943,25 @@
         <v>52</v>
       </c>
       <c r="V85" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AA85" t="s">
         <v>54</v>
       </c>
       <c r="AB85">
-        <v>118831</v>
+        <v>117232</v>
       </c>
       <c r="AC85" t="s">
         <v>55</v>
       </c>
+      <c r="AD85" t="s">
+        <v>65</v>
+      </c>
       <c r="AE85" t="s">
         <v>43</v>
       </c>
       <c r="AG85">
-        <v>9.0909089999999998E-2</v>
+        <v>0.125</v>
       </c>
       <c r="AH85" t="s">
         <v>56</v>
@@ -9940,13 +9970,16 @@
         <v>43</v>
       </c>
       <c r="AJ85">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="AK85">
         <v>1</v>
       </c>
       <c r="AL85" t="s">
         <v>57</v>
+      </c>
+      <c r="AM85" t="s">
+        <v>99</v>
       </c>
       <c r="AN85" t="s">
         <v>58</v>
@@ -9957,10 +9990,10 @@
     </row>
     <row r="86" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B86" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C86" t="s">
         <v>43</v>
@@ -9990,25 +10023,25 @@
         <v>46</v>
       </c>
       <c r="L86" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
       <c r="M86" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N86">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O86">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P86">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q86">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R86" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="S86" t="s">
         <v>50</v>
@@ -10022,17 +10055,11 @@
       <c r="V86" t="s">
         <v>61</v>
       </c>
-      <c r="W86" t="s">
-        <v>116</v>
-      </c>
-      <c r="X86" t="s">
-        <v>133</v>
-      </c>
       <c r="AA86" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB86">
-        <v>109191</v>
+        <v>103359</v>
       </c>
       <c r="AC86" t="s">
         <v>55</v>
@@ -10041,7 +10068,7 @@
         <v>43</v>
       </c>
       <c r="AG86">
-        <v>9.0909089999999998E-2</v>
+        <v>1</v>
       </c>
       <c r="AH86" t="s">
         <v>56</v>
@@ -10050,7 +10077,7 @@
         <v>43</v>
       </c>
       <c r="AJ86">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="AK86">
         <v>1</v>
@@ -10067,10 +10094,10 @@
     </row>
     <row r="87" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C87" t="s">
         <v>43</v>
@@ -10100,55 +10127,34 @@
         <v>46</v>
       </c>
       <c r="L87" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
       <c r="M87" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N87">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O87">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P87">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q87">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R87" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="S87" t="s">
-        <v>50</v>
-      </c>
-      <c r="T87" t="s">
-        <v>51</v>
-      </c>
-      <c r="U87" t="s">
-        <v>52</v>
-      </c>
-      <c r="V87" t="s">
-        <v>61</v>
-      </c>
-      <c r="W87" t="s">
-        <v>116</v>
-      </c>
-      <c r="X87" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y87" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z87" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="AA87" t="s">
         <v>54</v>
       </c>
       <c r="AB87">
-        <v>200660</v>
+        <v>202422</v>
       </c>
       <c r="AC87" t="s">
         <v>55</v>
@@ -10156,8 +10162,11 @@
       <c r="AE87" t="s">
         <v>43</v>
       </c>
+      <c r="AF87" t="s">
+        <v>129</v>
+      </c>
       <c r="AG87">
-        <v>6.0606060000000003E-2</v>
+        <v>1</v>
       </c>
       <c r="AH87" t="s">
         <v>56</v>
@@ -10166,7 +10175,7 @@
         <v>43</v>
       </c>
       <c r="AJ87">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="AK87">
         <v>1</v>
@@ -10246,25 +10255,22 @@
         <v>52</v>
       </c>
       <c r="V88" t="s">
-        <v>61</v>
-      </c>
-      <c r="W88" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="AA88" t="s">
         <v>54</v>
       </c>
       <c r="AB88">
-        <v>103358</v>
+        <v>109216</v>
       </c>
       <c r="AC88" t="s">
         <v>55</v>
       </c>
       <c r="AE88" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="AG88">
-        <v>9.0909089999999998E-2</v>
+        <v>0.18181820000000001</v>
       </c>
       <c r="AH88" t="s">
         <v>56</v>
@@ -10353,13 +10359,13 @@
         <v>52</v>
       </c>
       <c r="V89" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AA89" t="s">
         <v>54</v>
       </c>
       <c r="AB89">
-        <v>152741</v>
+        <v>118831</v>
       </c>
       <c r="AC89" t="s">
         <v>55</v>
@@ -10368,7 +10374,7 @@
         <v>43</v>
       </c>
       <c r="AG89">
-        <v>6.0606060000000003E-2</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH89" t="s">
         <v>56</v>
@@ -10457,25 +10463,28 @@
         <v>52</v>
       </c>
       <c r="V90" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="W90" t="s">
+        <v>116</v>
+      </c>
+      <c r="X90" t="s">
+        <v>133</v>
       </c>
       <c r="AA90" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB90">
-        <v>117232</v>
+        <v>109191</v>
       </c>
       <c r="AC90" t="s">
         <v>55</v>
       </c>
-      <c r="AD90" t="s">
-        <v>65</v>
-      </c>
       <c r="AE90" t="s">
         <v>43</v>
       </c>
       <c r="AG90">
-        <v>0.21212120000000001</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH90" t="s">
         <v>56</v>
@@ -10491,9 +10500,6 @@
       </c>
       <c r="AL90" t="s">
         <v>57</v>
-      </c>
-      <c r="AM90" t="s">
-        <v>99</v>
       </c>
       <c r="AN90" t="s">
         <v>58</v>
@@ -10566,23 +10572,35 @@
       <c r="U91" t="s">
         <v>52</v>
       </c>
+      <c r="V91" t="s">
+        <v>61</v>
+      </c>
+      <c r="W91" t="s">
+        <v>116</v>
+      </c>
+      <c r="X91" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>135</v>
+      </c>
       <c r="AA91" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB91">
-        <v>99208</v>
+        <v>200660</v>
       </c>
       <c r="AC91" t="s">
         <v>55</v>
       </c>
-      <c r="AD91" t="s">
-        <v>136</v>
-      </c>
       <c r="AE91" t="s">
         <v>43</v>
       </c>
       <c r="AG91">
-        <v>3.0303030000000002E-2</v>
+        <v>6.0606060000000003E-2</v>
       </c>
       <c r="AH91" t="s">
         <v>56</v>
@@ -10671,28 +10689,31 @@
         <v>52</v>
       </c>
       <c r="V92" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="W92" t="s">
+        <v>62</v>
       </c>
       <c r="AA92" t="s">
         <v>54</v>
       </c>
       <c r="AB92">
-        <v>109216</v>
+        <v>103358</v>
       </c>
       <c r="AC92" t="s">
         <v>55</v>
       </c>
       <c r="AE92" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="AG92">
-        <v>0.10833333333333334</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH92" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI92">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI92" t="s">
+        <v>43</v>
       </c>
       <c r="AJ92">
         <v>33</v>
@@ -10775,13 +10796,13 @@
         <v>52</v>
       </c>
       <c r="V93" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AA93" t="s">
         <v>54</v>
       </c>
       <c r="AB93">
-        <v>118831</v>
+        <v>152741</v>
       </c>
       <c r="AC93" t="s">
         <v>55</v>
@@ -10790,13 +10811,13 @@
         <v>43</v>
       </c>
       <c r="AG93">
-        <v>0.125</v>
+        <v>6.0606060000000003E-2</v>
       </c>
       <c r="AH93" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI93">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI93" t="s">
+        <v>43</v>
       </c>
       <c r="AJ93">
         <v>33</v>
@@ -10879,34 +10900,31 @@
         <v>52</v>
       </c>
       <c r="V94" t="s">
-        <v>61</v>
-      </c>
-      <c r="W94" t="s">
-        <v>116</v>
-      </c>
-      <c r="X94" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="AA94" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB94">
-        <v>109191</v>
+        <v>117232</v>
       </c>
       <c r="AC94" t="s">
         <v>55</v>
       </c>
+      <c r="AD94" t="s">
+        <v>65</v>
+      </c>
       <c r="AE94" t="s">
         <v>43</v>
       </c>
       <c r="AG94">
-        <v>0.33333333333333331</v>
+        <v>0.21212120000000001</v>
       </c>
       <c r="AH94" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI94">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI94" t="s">
+        <v>43</v>
       </c>
       <c r="AJ94">
         <v>33</v>
@@ -10916,6 +10934,9 @@
       </c>
       <c r="AL94" t="s">
         <v>57</v>
+      </c>
+      <c r="AM94" t="s">
+        <v>99</v>
       </c>
       <c r="AN94" t="s">
         <v>58</v>
@@ -10988,41 +11009,29 @@
       <c r="U95" t="s">
         <v>52</v>
       </c>
-      <c r="V95" t="s">
-        <v>61</v>
-      </c>
-      <c r="W95" t="s">
-        <v>116</v>
-      </c>
-      <c r="X95" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y95" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z95" t="s">
-        <v>135</v>
-      </c>
       <c r="AA95" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB95">
-        <v>200660</v>
+        <v>99208</v>
       </c>
       <c r="AC95" t="s">
         <v>55</v>
       </c>
+      <c r="AD95" t="s">
+        <v>136</v>
+      </c>
       <c r="AE95" t="s">
         <v>43</v>
       </c>
       <c r="AG95">
-        <v>1.6666666666666666E-2</v>
+        <v>3.0303030000000002E-2</v>
       </c>
       <c r="AH95" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI95">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI95" t="s">
+        <v>43</v>
       </c>
       <c r="AJ95">
         <v>33</v>
@@ -11105,25 +11114,22 @@
         <v>52</v>
       </c>
       <c r="V96" t="s">
-        <v>61</v>
-      </c>
-      <c r="W96" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="AA96" t="s">
         <v>54</v>
       </c>
       <c r="AB96">
-        <v>103358</v>
+        <v>109216</v>
       </c>
       <c r="AC96" t="s">
         <v>55</v>
       </c>
       <c r="AE96" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="AG96">
-        <v>0.29166666666666669</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="AH96" t="s">
         <v>90</v>
@@ -11141,7 +11147,7 @@
         <v>57</v>
       </c>
       <c r="AN96" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO96" t="s">
         <v>59</v>
@@ -11212,13 +11218,13 @@
         <v>52</v>
       </c>
       <c r="V97" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AA97" t="s">
         <v>54</v>
       </c>
       <c r="AB97">
-        <v>152741</v>
+        <v>118831</v>
       </c>
       <c r="AC97" t="s">
         <v>55</v>
@@ -11227,7 +11233,7 @@
         <v>43</v>
       </c>
       <c r="AG97">
-        <v>1.6666666666666666E-2</v>
+        <v>0.125</v>
       </c>
       <c r="AH97" t="s">
         <v>90</v>
@@ -11245,7 +11251,7 @@
         <v>57</v>
       </c>
       <c r="AN97" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO97" t="s">
         <v>59</v>
@@ -11316,25 +11322,28 @@
         <v>52</v>
       </c>
       <c r="V98" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="W98" t="s">
+        <v>116</v>
+      </c>
+      <c r="X98" t="s">
+        <v>133</v>
       </c>
       <c r="AA98" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB98">
-        <v>117232</v>
+        <v>109191</v>
       </c>
       <c r="AC98" t="s">
         <v>55</v>
       </c>
-      <c r="AD98" t="s">
-        <v>65</v>
-      </c>
       <c r="AE98" t="s">
         <v>43</v>
       </c>
       <c r="AG98">
-        <v>0.10833333333333334</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AH98" t="s">
         <v>90</v>
@@ -11351,11 +11360,8 @@
       <c r="AL98" t="s">
         <v>57</v>
       </c>
-      <c r="AM98" t="s">
-        <v>99</v>
-      </c>
       <c r="AN98" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO98" t="s">
         <v>59</v>
@@ -11425,23 +11431,35 @@
       <c r="U99" t="s">
         <v>52</v>
       </c>
+      <c r="V99" t="s">
+        <v>61</v>
+      </c>
+      <c r="W99" t="s">
+        <v>116</v>
+      </c>
+      <c r="X99" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y99" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z99" t="s">
+        <v>135</v>
+      </c>
       <c r="AA99" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB99">
-        <v>99208</v>
+        <v>200660</v>
       </c>
       <c r="AC99" t="s">
         <v>55</v>
       </c>
-      <c r="AD99" t="s">
-        <v>136</v>
-      </c>
       <c r="AE99" t="s">
         <v>43</v>
       </c>
       <c r="AG99">
-        <v>9.1666999999999998E-2</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="AH99" t="s">
         <v>90</v>
@@ -11459,7 +11477,7 @@
         <v>57</v>
       </c>
       <c r="AN99" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO99" t="s">
         <v>59</v>
@@ -11467,13 +11485,13 @@
     </row>
     <row r="100" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B100" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C100" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D100" t="s">
         <v>44</v>
@@ -11500,22 +11518,22 @@
         <v>46</v>
       </c>
       <c r="L100" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M100" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N100">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O100">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P100">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q100">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R100" t="s">
         <v>49</v>
@@ -11527,16 +11545,19 @@
         <v>51</v>
       </c>
       <c r="U100" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="V100" t="s">
-        <v>142</v>
+        <v>61</v>
+      </c>
+      <c r="W100" t="s">
+        <v>62</v>
       </c>
       <c r="AA100" t="s">
         <v>54</v>
       </c>
       <c r="AB100">
-        <v>82732</v>
+        <v>103358</v>
       </c>
       <c r="AC100" t="s">
         <v>55</v>
@@ -11545,16 +11566,16 @@
         <v>43</v>
       </c>
       <c r="AG100">
-        <v>4.7619050000000003E-2</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="AH100" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI100" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI100">
+        <v>131</v>
       </c>
       <c r="AJ100">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK100">
         <v>1</v>
@@ -11563,7 +11584,7 @@
         <v>57</v>
       </c>
       <c r="AN100" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO100" t="s">
         <v>59</v>
@@ -11571,13 +11592,13 @@
     </row>
     <row r="101" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B101" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C101" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D101" t="s">
         <v>44</v>
@@ -11604,22 +11625,22 @@
         <v>46</v>
       </c>
       <c r="L101" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M101" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N101">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O101">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P101">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q101">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R101" t="s">
         <v>49</v>
@@ -11634,13 +11655,13 @@
         <v>52</v>
       </c>
       <c r="V101" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="AA101" t="s">
         <v>54</v>
       </c>
       <c r="AB101">
-        <v>109216</v>
+        <v>152741</v>
       </c>
       <c r="AC101" t="s">
         <v>55</v>
@@ -11649,16 +11670,16 @@
         <v>43</v>
       </c>
       <c r="AG101">
-        <v>0.71428570000000002</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="AH101" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI101" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI101">
+        <v>131</v>
       </c>
       <c r="AJ101">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK101">
         <v>1</v>
@@ -11667,7 +11688,7 @@
         <v>57</v>
       </c>
       <c r="AN101" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO101" t="s">
         <v>59</v>
@@ -11675,13 +11696,13 @@
     </row>
     <row r="102" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B102" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C102" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D102" t="s">
         <v>44</v>
@@ -11708,22 +11729,22 @@
         <v>46</v>
       </c>
       <c r="L102" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M102" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N102">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O102">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P102">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q102">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R102" t="s">
         <v>49</v>
@@ -11738,31 +11759,34 @@
         <v>52</v>
       </c>
       <c r="V102" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AA102" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB102">
-        <v>118831</v>
+        <v>117232</v>
       </c>
       <c r="AC102" t="s">
         <v>55</v>
       </c>
+      <c r="AD102" t="s">
+        <v>65</v>
+      </c>
       <c r="AE102" t="s">
         <v>43</v>
       </c>
       <c r="AG102">
-        <v>0.23809520000000001</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="AH102" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI102" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI102">
+        <v>131</v>
       </c>
       <c r="AJ102">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK102">
         <v>1</v>
@@ -11770,8 +11794,11 @@
       <c r="AL102" t="s">
         <v>57</v>
       </c>
+      <c r="AM102" t="s">
+        <v>99</v>
+      </c>
       <c r="AN102" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO102" t="s">
         <v>59</v>
@@ -11779,13 +11806,13 @@
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B103" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C103" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D103" t="s">
         <v>44</v>
@@ -11812,22 +11839,22 @@
         <v>46</v>
       </c>
       <c r="L103" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M103" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N103">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O103">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P103">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q103">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R103" t="s">
         <v>49</v>
@@ -11841,20 +11868,11 @@
       <c r="U103" t="s">
         <v>52</v>
       </c>
-      <c r="V103" t="s">
-        <v>60</v>
-      </c>
-      <c r="W103" t="s">
-        <v>105</v>
-      </c>
-      <c r="X103" t="s">
-        <v>106</v>
-      </c>
       <c r="AA103" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB103">
-        <v>118840</v>
+        <v>99208</v>
       </c>
       <c r="AC103" t="s">
         <v>55</v>
@@ -11866,16 +11884,16 @@
         <v>43</v>
       </c>
       <c r="AG103">
-        <v>4.7619050000000003E-2</v>
+        <v>9.1666999999999998E-2</v>
       </c>
       <c r="AH103" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI103" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI103">
+        <v>131</v>
       </c>
       <c r="AJ103">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK103">
         <v>1</v>
@@ -11884,7 +11902,7 @@
         <v>57</v>
       </c>
       <c r="AN103" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO103" t="s">
         <v>59</v>
@@ -11952,22 +11970,16 @@
         <v>51</v>
       </c>
       <c r="U104" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="V104" t="s">
-        <v>63</v>
-      </c>
-      <c r="W104" t="s">
-        <v>96</v>
-      </c>
-      <c r="X104" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="AA104" t="s">
         <v>54</v>
       </c>
       <c r="AB104">
-        <v>153360</v>
+        <v>82732</v>
       </c>
       <c r="AC104" t="s">
         <v>55</v>
@@ -12065,28 +12077,22 @@
         <v>52</v>
       </c>
       <c r="V105" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AA105" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB105">
-        <v>117232</v>
+        <v>109216</v>
       </c>
       <c r="AC105" t="s">
         <v>55</v>
       </c>
-      <c r="AD105" t="s">
-        <v>67</v>
-      </c>
       <c r="AE105" t="s">
         <v>43</v>
       </c>
-      <c r="AF105" t="s">
-        <v>74</v>
-      </c>
       <c r="AG105">
-        <v>4.7619050000000003E-2</v>
+        <v>0.71428570000000002</v>
       </c>
       <c r="AH105" t="s">
         <v>56</v>
@@ -12175,34 +12181,22 @@
         <v>52</v>
       </c>
       <c r="V106" t="s">
-        <v>64</v>
-      </c>
-      <c r="X106" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y106" t="s">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="AA106" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB106">
-        <v>117478</v>
+        <v>118831</v>
       </c>
       <c r="AC106" t="s">
         <v>55</v>
       </c>
-      <c r="AD106" t="s">
-        <v>65</v>
-      </c>
       <c r="AE106" t="s">
         <v>43</v>
       </c>
-      <c r="AF106" t="s">
-        <v>145</v>
-      </c>
       <c r="AG106">
-        <v>9.5238089999999997E-2</v>
+        <v>0.23809520000000001</v>
       </c>
       <c r="AH106" t="s">
         <v>56</v>
@@ -12291,17 +12285,26 @@
         <v>52</v>
       </c>
       <c r="V107" t="s">
-        <v>75</v>
+        <v>60</v>
+      </c>
+      <c r="W107" t="s">
+        <v>105</v>
+      </c>
+      <c r="X107" t="s">
+        <v>106</v>
       </c>
       <c r="AA107" t="s">
         <v>54</v>
       </c>
       <c r="AB107">
-        <v>115095</v>
+        <v>118840</v>
       </c>
       <c r="AC107" t="s">
         <v>55</v>
       </c>
+      <c r="AD107" t="s">
+        <v>136</v>
+      </c>
       <c r="AE107" t="s">
         <v>43</v>
       </c>
@@ -12327,6 +12330,446 @@
         <v>58</v>
       </c>
       <c r="AO107" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>137</v>
+      </c>
+      <c r="B108" t="s">
+        <v>138</v>
+      </c>
+      <c r="C108" t="s">
+        <v>139</v>
+      </c>
+      <c r="D108" t="s">
+        <v>44</v>
+      </c>
+      <c r="E108" t="s">
+        <v>45</v>
+      </c>
+      <c r="F108" t="s">
+        <v>43</v>
+      </c>
+      <c r="G108" t="s">
+        <v>43</v>
+      </c>
+      <c r="H108" t="s">
+        <v>43</v>
+      </c>
+      <c r="I108" t="s">
+        <v>43</v>
+      </c>
+      <c r="J108" t="s">
+        <v>43</v>
+      </c>
+      <c r="K108" t="s">
+        <v>46</v>
+      </c>
+      <c r="L108" t="s">
+        <v>140</v>
+      </c>
+      <c r="M108" t="s">
+        <v>141</v>
+      </c>
+      <c r="N108">
+        <v>7</v>
+      </c>
+      <c r="O108">
+        <v>1876</v>
+      </c>
+      <c r="P108">
+        <v>7</v>
+      </c>
+      <c r="Q108">
+        <v>1876</v>
+      </c>
+      <c r="R108" t="s">
+        <v>49</v>
+      </c>
+      <c r="S108" t="s">
+        <v>50</v>
+      </c>
+      <c r="T108" t="s">
+        <v>51</v>
+      </c>
+      <c r="U108" t="s">
+        <v>52</v>
+      </c>
+      <c r="V108" t="s">
+        <v>63</v>
+      </c>
+      <c r="W108" t="s">
+        <v>96</v>
+      </c>
+      <c r="X108" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB108">
+        <v>153360</v>
+      </c>
+      <c r="AC108" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE108" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG108">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH108" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI108" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ108">
+        <v>21</v>
+      </c>
+      <c r="AK108">
+        <v>1</v>
+      </c>
+      <c r="AL108" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN108" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>137</v>
+      </c>
+      <c r="B109" t="s">
+        <v>138</v>
+      </c>
+      <c r="C109" t="s">
+        <v>139</v>
+      </c>
+      <c r="D109" t="s">
+        <v>44</v>
+      </c>
+      <c r="E109" t="s">
+        <v>45</v>
+      </c>
+      <c r="F109" t="s">
+        <v>43</v>
+      </c>
+      <c r="G109" t="s">
+        <v>43</v>
+      </c>
+      <c r="H109" t="s">
+        <v>43</v>
+      </c>
+      <c r="I109" t="s">
+        <v>43</v>
+      </c>
+      <c r="J109" t="s">
+        <v>43</v>
+      </c>
+      <c r="K109" t="s">
+        <v>46</v>
+      </c>
+      <c r="L109" t="s">
+        <v>140</v>
+      </c>
+      <c r="M109" t="s">
+        <v>141</v>
+      </c>
+      <c r="N109">
+        <v>7</v>
+      </c>
+      <c r="O109">
+        <v>1876</v>
+      </c>
+      <c r="P109">
+        <v>7</v>
+      </c>
+      <c r="Q109">
+        <v>1876</v>
+      </c>
+      <c r="R109" t="s">
+        <v>49</v>
+      </c>
+      <c r="S109" t="s">
+        <v>50</v>
+      </c>
+      <c r="T109" t="s">
+        <v>51</v>
+      </c>
+      <c r="U109" t="s">
+        <v>52</v>
+      </c>
+      <c r="V109" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB109">
+        <v>117232</v>
+      </c>
+      <c r="AC109" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD109" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE109" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF109" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG109">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH109" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI109" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ109">
+        <v>21</v>
+      </c>
+      <c r="AK109">
+        <v>1</v>
+      </c>
+      <c r="AL109" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN109" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO109" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>137</v>
+      </c>
+      <c r="B110" t="s">
+        <v>138</v>
+      </c>
+      <c r="C110" t="s">
+        <v>139</v>
+      </c>
+      <c r="D110" t="s">
+        <v>44</v>
+      </c>
+      <c r="E110" t="s">
+        <v>45</v>
+      </c>
+      <c r="F110" t="s">
+        <v>43</v>
+      </c>
+      <c r="G110" t="s">
+        <v>43</v>
+      </c>
+      <c r="H110" t="s">
+        <v>43</v>
+      </c>
+      <c r="I110" t="s">
+        <v>43</v>
+      </c>
+      <c r="J110" t="s">
+        <v>43</v>
+      </c>
+      <c r="K110" t="s">
+        <v>46</v>
+      </c>
+      <c r="L110" t="s">
+        <v>140</v>
+      </c>
+      <c r="M110" t="s">
+        <v>141</v>
+      </c>
+      <c r="N110">
+        <v>7</v>
+      </c>
+      <c r="O110">
+        <v>1876</v>
+      </c>
+      <c r="P110">
+        <v>7</v>
+      </c>
+      <c r="Q110">
+        <v>1876</v>
+      </c>
+      <c r="R110" t="s">
+        <v>49</v>
+      </c>
+      <c r="S110" t="s">
+        <v>50</v>
+      </c>
+      <c r="T110" t="s">
+        <v>51</v>
+      </c>
+      <c r="U110" t="s">
+        <v>52</v>
+      </c>
+      <c r="V110" t="s">
+        <v>64</v>
+      </c>
+      <c r="X110" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y110" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA110" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB110">
+        <v>117478</v>
+      </c>
+      <c r="AC110" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD110" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE110" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF110" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG110">
+        <v>9.5238089999999997E-2</v>
+      </c>
+      <c r="AH110" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI110" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ110">
+        <v>21</v>
+      </c>
+      <c r="AK110">
+        <v>1</v>
+      </c>
+      <c r="AL110" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN110" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO110" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>137</v>
+      </c>
+      <c r="B111" t="s">
+        <v>138</v>
+      </c>
+      <c r="C111" t="s">
+        <v>139</v>
+      </c>
+      <c r="D111" t="s">
+        <v>44</v>
+      </c>
+      <c r="E111" t="s">
+        <v>45</v>
+      </c>
+      <c r="F111" t="s">
+        <v>43</v>
+      </c>
+      <c r="G111" t="s">
+        <v>43</v>
+      </c>
+      <c r="H111" t="s">
+        <v>43</v>
+      </c>
+      <c r="I111" t="s">
+        <v>43</v>
+      </c>
+      <c r="J111" t="s">
+        <v>43</v>
+      </c>
+      <c r="K111" t="s">
+        <v>46</v>
+      </c>
+      <c r="L111" t="s">
+        <v>140</v>
+      </c>
+      <c r="M111" t="s">
+        <v>141</v>
+      </c>
+      <c r="N111">
+        <v>7</v>
+      </c>
+      <c r="O111">
+        <v>1876</v>
+      </c>
+      <c r="P111">
+        <v>7</v>
+      </c>
+      <c r="Q111">
+        <v>1876</v>
+      </c>
+      <c r="R111" t="s">
+        <v>49</v>
+      </c>
+      <c r="S111" t="s">
+        <v>50</v>
+      </c>
+      <c r="T111" t="s">
+        <v>51</v>
+      </c>
+      <c r="U111" t="s">
+        <v>52</v>
+      </c>
+      <c r="V111" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA111" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB111">
+        <v>115095</v>
+      </c>
+      <c r="AC111" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE111" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG111">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH111" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI111" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ111">
+        <v>21</v>
+      </c>
+      <c r="AK111">
+        <v>1</v>
+      </c>
+      <c r="AL111" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN111" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO111" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added items for bay-breasted yellow warbler
</commit_message>
<xml_diff>
--- a/AvianDietDatabase_King_1883_AD.xlsx
+++ b/AvianDietDatabase_King_1883_AD.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="155">
   <si>
     <t>Common_Name</t>
   </si>
@@ -829,9 +829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM64" sqref="AM64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO19" sqref="AO19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>43</v>
@@ -1784,19 +1784,19 @@
         <v>47</v>
       </c>
       <c r="M9" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="N9">
         <v>7</v>
       </c>
       <c r="O9">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P9">
         <v>7</v>
       </c>
       <c r="Q9">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R9" t="s">
         <v>49</v>
@@ -1826,16 +1826,16 @@
         <v>43</v>
       </c>
       <c r="AG9">
-        <v>0.35294120000000001</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="AH9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI9">
+        <v>42</v>
       </c>
       <c r="AJ9">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AK9">
         <v>1</v>
@@ -1844,7 +1844,7 @@
         <v>57</v>
       </c>
       <c r="AN9" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO9" t="s">
         <v>59</v>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
@@ -1888,19 +1888,19 @@
         <v>47</v>
       </c>
       <c r="M10" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="N10">
         <v>7</v>
       </c>
       <c r="O10">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P10">
         <v>7</v>
       </c>
       <c r="Q10">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R10" t="s">
         <v>49</v>
@@ -1930,16 +1930,16 @@
         <v>43</v>
       </c>
       <c r="AG10">
-        <v>0.17647060000000001</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="AH10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI10">
+        <v>42</v>
       </c>
       <c r="AJ10">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AK10">
         <v>1</v>
@@ -1948,7 +1948,7 @@
         <v>57</v>
       </c>
       <c r="AN10" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO10" t="s">
         <v>59</v>
@@ -1956,10 +1956,10 @@
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>43</v>
@@ -1992,19 +1992,19 @@
         <v>47</v>
       </c>
       <c r="M11" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="N11">
         <v>7</v>
       </c>
       <c r="O11">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P11">
         <v>7</v>
       </c>
       <c r="Q11">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R11" t="s">
         <v>49</v>
@@ -2037,16 +2037,16 @@
         <v>43</v>
       </c>
       <c r="AG11">
-        <v>0.1176471</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="AH11" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI11">
+        <v>42</v>
       </c>
       <c r="AJ11">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AK11">
         <v>1</v>
@@ -2055,7 +2055,7 @@
         <v>57</v>
       </c>
       <c r="AN11" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO11" t="s">
         <v>59</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>43</v>
@@ -2099,19 +2099,19 @@
         <v>47</v>
       </c>
       <c r="M12" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="O12">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P12">
         <v>7</v>
       </c>
       <c r="Q12">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R12" t="s">
         <v>49</v>
@@ -2141,16 +2141,16 @@
         <v>43</v>
       </c>
       <c r="AG12">
-        <v>0.17647060000000001</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="AH12" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI12">
+        <v>42</v>
       </c>
       <c r="AJ12">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AK12">
         <v>1</v>
@@ -2159,7 +2159,7 @@
         <v>57</v>
       </c>
       <c r="AN12" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO12" t="s">
         <v>59</v>
@@ -2167,10 +2167,10 @@
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>43</v>
@@ -2203,19 +2203,19 @@
         <v>47</v>
       </c>
       <c r="M13" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="N13">
         <v>7</v>
       </c>
       <c r="O13">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P13">
         <v>7</v>
       </c>
       <c r="Q13">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R13" t="s">
         <v>49</v>
@@ -2248,19 +2248,19 @@
         <v>43</v>
       </c>
       <c r="AF13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="AG13">
-        <v>0.1176471</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="AH13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI13">
+        <v>42</v>
       </c>
       <c r="AJ13">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AK13">
         <v>1</v>
@@ -2269,7 +2269,7 @@
         <v>57</v>
       </c>
       <c r="AN13" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO13" t="s">
         <v>59</v>
@@ -2277,10 +2277,10 @@
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
@@ -2313,19 +2313,19 @@
         <v>47</v>
       </c>
       <c r="M14" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="N14">
         <v>7</v>
       </c>
       <c r="O14">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P14">
         <v>7</v>
       </c>
       <c r="Q14">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R14" t="s">
         <v>49</v>
@@ -2358,19 +2358,19 @@
         <v>43</v>
       </c>
       <c r="AF14" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="AG14">
-        <v>0.17647060000000001</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="AH14" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI14">
+        <v>42</v>
       </c>
       <c r="AJ14">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AK14">
         <v>1</v>
@@ -2379,7 +2379,7 @@
         <v>57</v>
       </c>
       <c r="AN14" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO14" t="s">
         <v>59</v>
@@ -2387,10 +2387,10 @@
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>43</v>
@@ -2423,19 +2423,19 @@
         <v>47</v>
       </c>
       <c r="M15" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="N15">
         <v>7</v>
       </c>
       <c r="O15">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P15">
         <v>7</v>
       </c>
       <c r="Q15">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R15" t="s">
         <v>49</v>
@@ -2450,13 +2450,13 @@
         <v>52</v>
       </c>
       <c r="V15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="AA15" t="s">
         <v>54</v>
       </c>
       <c r="AB15">
-        <v>115095</v>
+        <v>101593</v>
       </c>
       <c r="AC15" t="s">
         <v>55</v>
@@ -2464,20 +2464,17 @@
       <c r="AE15" t="s">
         <v>43</v>
       </c>
-      <c r="AF15" t="s">
-        <v>76</v>
-      </c>
       <c r="AG15">
-        <v>5.8823529999999999E-2</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="AH15" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI15">
+        <v>42</v>
       </c>
       <c r="AJ15">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AK15">
         <v>1</v>
@@ -2486,7 +2483,7 @@
         <v>57</v>
       </c>
       <c r="AN15" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO15" t="s">
         <v>59</v>
@@ -2581,10 +2578,10 @@
         <v>5.8823529999999999E-2</v>
       </c>
       <c r="AH16" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI16" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI16">
+        <v>42</v>
       </c>
       <c r="AJ16">
         <v>17</v>
@@ -2596,7 +2593,7 @@
         <v>57</v>
       </c>
       <c r="AN16" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="AO16" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
added scientific name for blue eyed yellow warbler
</commit_message>
<xml_diff>
--- a/AvianDietDatabase_King_1883_AD.xlsx
+++ b/AvianDietDatabase_King_1883_AD.xlsx
@@ -496,9 +496,6 @@
     <t>Blue-eyed Yellow Warbler</t>
   </si>
   <si>
-    <t>Dendroica aestiva</t>
-  </si>
-  <si>
     <t>insect larvae</t>
   </si>
   <si>
@@ -506,6 +503,9 @@
   </si>
   <si>
     <t>AHD</t>
+  </si>
+  <si>
+    <t>Setophaga petechia</t>
   </si>
 </sst>
 </file>
@@ -830,8 +830,8 @@
   <dimension ref="A1:AO111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO19" sqref="AO19"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,7 +1844,7 @@
         <v>57</v>
       </c>
       <c r="AN9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO9" t="s">
         <v>59</v>
@@ -1948,7 +1948,7 @@
         <v>57</v>
       </c>
       <c r="AN10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO10" t="s">
         <v>59</v>
@@ -2055,7 +2055,7 @@
         <v>57</v>
       </c>
       <c r="AN11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO11" t="s">
         <v>59</v>
@@ -2159,7 +2159,7 @@
         <v>57</v>
       </c>
       <c r="AN12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO12" t="s">
         <v>59</v>
@@ -2269,7 +2269,7 @@
         <v>57</v>
       </c>
       <c r="AN13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO13" t="s">
         <v>59</v>
@@ -2379,7 +2379,7 @@
         <v>57</v>
       </c>
       <c r="AN14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO14" t="s">
         <v>59</v>
@@ -2483,7 +2483,7 @@
         <v>57</v>
       </c>
       <c r="AN15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO15" t="s">
         <v>59</v>
@@ -2593,7 +2593,7 @@
         <v>57</v>
       </c>
       <c r="AN16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO16" t="s">
         <v>59</v>
@@ -2697,7 +2697,7 @@
         <v>57</v>
       </c>
       <c r="AN17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO17" t="s">
         <v>59</v>
@@ -2801,7 +2801,7 @@
         <v>57</v>
       </c>
       <c r="AN18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO18" t="s">
         <v>59</v>
@@ -2908,7 +2908,7 @@
         <v>57</v>
       </c>
       <c r="AN19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO19" t="s">
         <v>59</v>
@@ -3012,7 +3012,7 @@
         <v>57</v>
       </c>
       <c r="AN20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO20" t="s">
         <v>59</v>
@@ -3122,7 +3122,7 @@
         <v>57</v>
       </c>
       <c r="AN21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO21" t="s">
         <v>59</v>
@@ -3232,7 +3232,7 @@
         <v>57</v>
       </c>
       <c r="AN22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO22" t="s">
         <v>59</v>
@@ -3339,7 +3339,7 @@
         <v>57</v>
       </c>
       <c r="AN23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO23" t="s">
         <v>59</v>
@@ -3449,7 +3449,7 @@
         <v>57</v>
       </c>
       <c r="AN24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO24" t="s">
         <v>59</v>
@@ -6991,7 +6991,7 @@
         <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C58" t="s">
         <v>43</v>
@@ -7024,7 +7024,7 @@
         <v>47</v>
       </c>
       <c r="M58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N58">
         <v>7</v>
@@ -7087,7 +7087,7 @@
         <v>57</v>
       </c>
       <c r="AN58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO58" t="s">
         <v>59</v>
@@ -7098,7 +7098,7 @@
         <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C59" t="s">
         <v>43</v>
@@ -7131,7 +7131,7 @@
         <v>47</v>
       </c>
       <c r="M59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N59">
         <v>7</v>
@@ -7173,7 +7173,7 @@
         <v>43</v>
       </c>
       <c r="AF59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG59">
         <v>0.5</v>
@@ -7194,7 +7194,7 @@
         <v>57</v>
       </c>
       <c r="AN59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO59" t="s">
         <v>59</v>
@@ -7205,7 +7205,7 @@
         <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s">
         <v>43</v>
@@ -7238,7 +7238,7 @@
         <v>47</v>
       </c>
       <c r="M60" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N60">
         <v>7</v>
@@ -7301,7 +7301,7 @@
         <v>57</v>
       </c>
       <c r="AN60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO60" t="s">
         <v>59</v>
@@ -7312,7 +7312,7 @@
         <v>150</v>
       </c>
       <c r="B61" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
         <v>43</v>
@@ -7345,7 +7345,7 @@
         <v>47</v>
       </c>
       <c r="M61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N61">
         <v>7</v>
@@ -7387,7 +7387,7 @@
         <v>43</v>
       </c>
       <c r="AF61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG61">
         <v>0.4</v>
@@ -7408,7 +7408,7 @@
         <v>57</v>
       </c>
       <c r="AN61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO61" t="s">
         <v>59</v>
@@ -8157,7 +8157,7 @@
         <v>57</v>
       </c>
       <c r="AN68" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO68" t="s">
         <v>59</v>
@@ -8267,7 +8267,7 @@
         <v>57</v>
       </c>
       <c r="AN69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO69" t="s">
         <v>59</v>
@@ -8380,7 +8380,7 @@
         <v>57</v>
       </c>
       <c r="AN70" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO70" t="s">
         <v>59</v>
@@ -8487,7 +8487,7 @@
         <v>57</v>
       </c>
       <c r="AN71" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO71" t="s">
         <v>59</v>
@@ -8597,7 +8597,7 @@
         <v>57</v>
       </c>
       <c r="AN72" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO72" t="s">
         <v>59</v>
@@ -8704,7 +8704,7 @@
         <v>57</v>
       </c>
       <c r="AN73" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO73" t="s">
         <v>59</v>
@@ -11144,7 +11144,7 @@
         <v>57</v>
       </c>
       <c r="AN96" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO96" t="s">
         <v>59</v>
@@ -11248,7 +11248,7 @@
         <v>57</v>
       </c>
       <c r="AN97" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO97" t="s">
         <v>59</v>
@@ -11358,7 +11358,7 @@
         <v>57</v>
       </c>
       <c r="AN98" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO98" t="s">
         <v>59</v>
@@ -11474,7 +11474,7 @@
         <v>57</v>
       </c>
       <c r="AN99" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO99" t="s">
         <v>59</v>
@@ -11581,7 +11581,7 @@
         <v>57</v>
       </c>
       <c r="AN100" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO100" t="s">
         <v>59</v>
@@ -11685,7 +11685,7 @@
         <v>57</v>
       </c>
       <c r="AN101" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO101" t="s">
         <v>59</v>
@@ -11795,7 +11795,7 @@
         <v>99</v>
       </c>
       <c r="AN102" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO102" t="s">
         <v>59</v>
@@ -11899,7 +11899,7 @@
         <v>57</v>
       </c>
       <c r="AN103" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AO103" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
black and yellow, palm, and pine warbler item/occurrence audited/entered
</commit_message>
<xml_diff>
--- a/AvianDietDatabase_King_1883_AD.xlsx
+++ b/AvianDietDatabase_King_1883_AD.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="AvianDietDatabase_King_1883" localSheetId="0">Sheet1!$A$1:$AO$111</definedName>
+    <definedName name="AvianDietDatabase_King_1883" localSheetId="0">Sheet1!$A$1:$AO$124</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2955" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3298" uniqueCount="155">
   <si>
     <t>Common_Name</t>
   </si>
@@ -512,10 +512,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,8 +548,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,11 +835,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO111"/>
+  <dimension ref="A1:AO124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A20" sqref="A20"/>
+      <selection pane="topRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8775,19 +8783,28 @@
         <v>52</v>
       </c>
       <c r="V74" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="W74" t="s">
+        <v>105</v>
+      </c>
+      <c r="X74" t="s">
+        <v>106</v>
       </c>
       <c r="AA74" t="s">
         <v>54</v>
       </c>
       <c r="AB74">
-        <v>109216</v>
+        <v>118831</v>
       </c>
       <c r="AC74" t="s">
         <v>55</v>
       </c>
       <c r="AE74" t="s">
         <v>43</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>115</v>
       </c>
       <c r="AG74">
         <v>0.35294120000000001</v>
@@ -8879,13 +8896,13 @@
         <v>52</v>
       </c>
       <c r="V75" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AA75" t="s">
         <v>54</v>
       </c>
       <c r="AB75">
-        <v>118831</v>
+        <v>152741</v>
       </c>
       <c r="AC75" t="s">
         <v>55</v>
@@ -8893,8 +8910,11 @@
       <c r="AE75" t="s">
         <v>43</v>
       </c>
+      <c r="AF75" t="s">
+        <v>146</v>
+      </c>
       <c r="AG75">
-        <v>0.35294120000000001</v>
+        <v>0.17647058823529413</v>
       </c>
       <c r="AH75" t="s">
         <v>56</v>
@@ -8983,13 +9003,13 @@
         <v>52</v>
       </c>
       <c r="V76" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA76" t="s">
         <v>54</v>
       </c>
       <c r="AB76">
-        <v>152741</v>
+        <v>109216</v>
       </c>
       <c r="AC76" t="s">
         <v>55</v>
@@ -8998,7 +9018,7 @@
         <v>43</v>
       </c>
       <c r="AG76">
-        <v>0.23529410000000001</v>
+        <v>0.35294120000000001</v>
       </c>
       <c r="AH76" t="s">
         <v>56</v>
@@ -9087,28 +9107,22 @@
         <v>52</v>
       </c>
       <c r="V77" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AA77" t="s">
         <v>54</v>
       </c>
       <c r="AB77">
-        <v>117232</v>
+        <v>118831</v>
       </c>
       <c r="AC77" t="s">
         <v>55</v>
       </c>
-      <c r="AD77" t="s">
-        <v>65</v>
-      </c>
       <c r="AE77" t="s">
         <v>43</v>
       </c>
-      <c r="AF77" t="s">
-        <v>66</v>
-      </c>
       <c r="AG77">
-        <v>5.8823529999999999E-2</v>
+        <v>0.35294120000000001</v>
       </c>
       <c r="AH77" t="s">
         <v>56</v>
@@ -9197,28 +9211,22 @@
         <v>52</v>
       </c>
       <c r="V78" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA78" t="s">
         <v>54</v>
       </c>
       <c r="AB78">
-        <v>117232</v>
+        <v>152741</v>
       </c>
       <c r="AC78" t="s">
         <v>55</v>
       </c>
-      <c r="AD78" t="s">
-        <v>67</v>
-      </c>
       <c r="AE78" t="s">
         <v>43</v>
       </c>
-      <c r="AF78" t="s">
-        <v>68</v>
-      </c>
       <c r="AG78">
-        <v>0.35294120000000001</v>
+        <v>0.17647058823529413</v>
       </c>
       <c r="AH78" t="s">
         <v>56</v>
@@ -9244,10 +9252,10 @@
     </row>
     <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C79" t="s">
         <v>43</v>
@@ -9277,22 +9285,22 @@
         <v>46</v>
       </c>
       <c r="L79" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M79" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="N79">
         <v>7</v>
       </c>
       <c r="O79">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P79">
         <v>7</v>
       </c>
       <c r="Q79">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R79" t="s">
         <v>49</v>
@@ -9325,10 +9333,10 @@
         <v>43</v>
       </c>
       <c r="AF79" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="AG79">
-        <v>1</v>
+        <v>0.35294117647058826</v>
       </c>
       <c r="AH79" t="s">
         <v>56</v>
@@ -9337,7 +9345,7 @@
         <v>43</v>
       </c>
       <c r="AJ79">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="AK79">
         <v>1</v>
@@ -9354,10 +9362,10 @@
     </row>
     <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C80" t="s">
         <v>43</v>
@@ -9387,22 +9395,22 @@
         <v>46</v>
       </c>
       <c r="L80" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="M80" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="N80">
         <v>7</v>
       </c>
       <c r="O80">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="P80">
         <v>7</v>
       </c>
       <c r="Q80">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="R80" t="s">
         <v>49</v>
@@ -9416,23 +9424,29 @@
       <c r="U80" t="s">
         <v>52</v>
       </c>
+      <c r="V80" t="s">
+        <v>64</v>
+      </c>
       <c r="AA80" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB80">
-        <v>99208</v>
+        <v>117232</v>
       </c>
       <c r="AC80" t="s">
         <v>55</v>
       </c>
+      <c r="AD80" t="s">
+        <v>67</v>
+      </c>
       <c r="AE80" t="s">
         <v>43</v>
       </c>
       <c r="AF80" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="AG80">
-        <v>1</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="AH80" t="s">
         <v>56</v>
@@ -9441,7 +9455,7 @@
         <v>43</v>
       </c>
       <c r="AJ80">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="AK80">
         <v>1</v>
@@ -9458,10 +9472,10 @@
     </row>
     <row r="81" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C81" t="s">
         <v>43</v>
@@ -9500,13 +9514,13 @@
         <v>7</v>
       </c>
       <c r="O81">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P81">
         <v>7</v>
       </c>
       <c r="Q81">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R81" t="s">
         <v>49</v>
@@ -9521,13 +9535,19 @@
         <v>52</v>
       </c>
       <c r="V81" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="W81" t="s">
+        <v>105</v>
+      </c>
+      <c r="X81" t="s">
+        <v>106</v>
       </c>
       <c r="AA81" t="s">
         <v>54</v>
       </c>
       <c r="AB81">
-        <v>109216</v>
+        <v>118831</v>
       </c>
       <c r="AC81" t="s">
         <v>55</v>
@@ -9535,17 +9555,20 @@
       <c r="AE81" t="s">
         <v>43</v>
       </c>
+      <c r="AF81" t="s">
+        <v>115</v>
+      </c>
       <c r="AG81">
-        <v>0.25</v>
+        <v>4.0816326530612242E-2</v>
       </c>
       <c r="AH81" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI81" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI81">
+        <v>36</v>
       </c>
       <c r="AJ81">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AK81">
         <v>1</v>
@@ -9562,10 +9585,10 @@
     </row>
     <row r="82" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B82" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C82" t="s">
         <v>43</v>
@@ -9604,13 +9627,13 @@
         <v>7</v>
       </c>
       <c r="O82">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P82">
         <v>7</v>
       </c>
       <c r="Q82">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R82" t="s">
         <v>49</v>
@@ -9625,13 +9648,13 @@
         <v>52</v>
       </c>
       <c r="V82" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AA82" t="s">
         <v>54</v>
       </c>
       <c r="AB82">
-        <v>118831</v>
+        <v>152741</v>
       </c>
       <c r="AC82" t="s">
         <v>55</v>
@@ -9639,17 +9662,20 @@
       <c r="AE82" t="s">
         <v>43</v>
       </c>
+      <c r="AF82" t="s">
+        <v>146</v>
+      </c>
       <c r="AG82">
-        <v>0.125</v>
+        <v>4.0816326530612242E-2</v>
       </c>
       <c r="AH82" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI82" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI82">
+        <v>36</v>
       </c>
       <c r="AJ82">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AK82">
         <v>1</v>
@@ -9666,10 +9692,10 @@
     </row>
     <row r="83" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B83" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C83" t="s">
         <v>43</v>
@@ -9708,13 +9734,13 @@
         <v>7</v>
       </c>
       <c r="O83">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P83">
         <v>7</v>
       </c>
       <c r="Q83">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R83" t="s">
         <v>49</v>
@@ -9729,16 +9755,13 @@
         <v>52</v>
       </c>
       <c r="V83" t="s">
-        <v>61</v>
-      </c>
-      <c r="W83" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="AA83" t="s">
         <v>54</v>
       </c>
       <c r="AB83">
-        <v>103358</v>
+        <v>109216</v>
       </c>
       <c r="AC83" t="s">
         <v>55</v>
@@ -9747,16 +9770,16 @@
         <v>43</v>
       </c>
       <c r="AG83">
-        <v>0.125</v>
+        <v>0.24489795918367346</v>
       </c>
       <c r="AH83" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI83" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI83">
+        <v>36</v>
       </c>
       <c r="AJ83">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AK83">
         <v>1</v>
@@ -9773,10 +9796,10 @@
     </row>
     <row r="84" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B84" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C84" t="s">
         <v>43</v>
@@ -9815,13 +9838,13 @@
         <v>7</v>
       </c>
       <c r="O84">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P84">
         <v>7</v>
       </c>
       <c r="Q84">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R84" t="s">
         <v>49</v>
@@ -9836,13 +9859,13 @@
         <v>52</v>
       </c>
       <c r="V84" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AA84" t="s">
         <v>54</v>
       </c>
       <c r="AB84">
-        <v>152741</v>
+        <v>118831</v>
       </c>
       <c r="AC84" t="s">
         <v>55</v>
@@ -9851,16 +9874,16 @@
         <v>43</v>
       </c>
       <c r="AG84">
-        <v>0.125</v>
+        <v>0.26530612244897961</v>
       </c>
       <c r="AH84" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI84" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI84">
+        <v>36</v>
       </c>
       <c r="AJ84">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AK84">
         <v>1</v>
@@ -9877,10 +9900,10 @@
     </row>
     <row r="85" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B85" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C85" t="s">
         <v>43</v>
@@ -9919,13 +9942,13 @@
         <v>7</v>
       </c>
       <c r="O85">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P85">
         <v>7</v>
       </c>
       <c r="Q85">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R85" t="s">
         <v>49</v>
@@ -9940,43 +9963,37 @@
         <v>52</v>
       </c>
       <c r="V85" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA85" t="s">
         <v>54</v>
       </c>
       <c r="AB85">
-        <v>117232</v>
+        <v>152741</v>
       </c>
       <c r="AC85" t="s">
         <v>55</v>
       </c>
-      <c r="AD85" t="s">
-        <v>65</v>
-      </c>
       <c r="AE85" t="s">
         <v>43</v>
       </c>
       <c r="AG85">
-        <v>0.125</v>
+        <v>4.0816326530612242E-2</v>
       </c>
       <c r="AH85" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI85" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI85">
+        <v>36</v>
       </c>
       <c r="AJ85">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="AK85">
         <v>1</v>
       </c>
       <c r="AL85" t="s">
         <v>57</v>
-      </c>
-      <c r="AM85" t="s">
-        <v>99</v>
       </c>
       <c r="AN85" t="s">
         <v>58</v>
@@ -9987,10 +10004,10 @@
     </row>
     <row r="86" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C86" t="s">
         <v>43</v>
@@ -10020,25 +10037,25 @@
         <v>46</v>
       </c>
       <c r="L86" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="M86" t="s">
         <v>89</v>
       </c>
       <c r="N86">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O86">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P86">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q86">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R86" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="S86" t="s">
         <v>50</v>
@@ -10050,31 +10067,37 @@
         <v>52</v>
       </c>
       <c r="V86" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AA86" t="s">
         <v>54</v>
       </c>
       <c r="AB86">
-        <v>103359</v>
+        <v>117232</v>
       </c>
       <c r="AC86" t="s">
         <v>55</v>
       </c>
+      <c r="AD86" t="s">
+        <v>65</v>
+      </c>
       <c r="AE86" t="s">
         <v>43</v>
       </c>
+      <c r="AF86" t="s">
+        <v>66</v>
+      </c>
       <c r="AG86">
-        <v>1</v>
+        <v>0.34693877551020408</v>
       </c>
       <c r="AH86" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI86" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI86">
+        <v>36</v>
       </c>
       <c r="AJ86">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="AK86">
         <v>1</v>
@@ -10091,10 +10114,10 @@
     </row>
     <row r="87" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B87" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C87" t="s">
         <v>43</v>
@@ -10124,55 +10147,67 @@
         <v>46</v>
       </c>
       <c r="L87" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="M87" t="s">
         <v>89</v>
       </c>
       <c r="N87">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O87">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="P87">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q87">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="R87" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="S87" t="s">
-        <v>128</v>
+        <v>50</v>
+      </c>
+      <c r="T87" t="s">
+        <v>51</v>
+      </c>
+      <c r="U87" t="s">
+        <v>52</v>
+      </c>
+      <c r="V87" t="s">
+        <v>64</v>
       </c>
       <c r="AA87" t="s">
         <v>54</v>
       </c>
       <c r="AB87">
-        <v>202422</v>
+        <v>117232</v>
       </c>
       <c r="AC87" t="s">
         <v>55</v>
       </c>
+      <c r="AD87" t="s">
+        <v>67</v>
+      </c>
       <c r="AE87" t="s">
         <v>43</v>
       </c>
       <c r="AF87" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="AG87">
-        <v>1</v>
+        <v>2.0408163265306121E-2</v>
       </c>
       <c r="AH87" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI87" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI87">
+        <v>36</v>
       </c>
       <c r="AJ87">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="AK87">
         <v>1</v>
@@ -10189,10 +10224,10 @@
     </row>
     <row r="88" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B88" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C88" t="s">
         <v>43</v>
@@ -10222,22 +10257,22 @@
         <v>46</v>
       </c>
       <c r="L88" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="M88" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="N88">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O88">
-        <v>1877</v>
+        <v>1873</v>
       </c>
       <c r="P88">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q88">
-        <v>1877</v>
+        <v>1873</v>
       </c>
       <c r="R88" t="s">
         <v>49</v>
@@ -10251,23 +10286,23 @@
       <c r="U88" t="s">
         <v>52</v>
       </c>
-      <c r="V88" t="s">
-        <v>53</v>
-      </c>
       <c r="AA88" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB88">
-        <v>109216</v>
+        <v>99208</v>
       </c>
       <c r="AC88" t="s">
         <v>55</v>
       </c>
       <c r="AE88" t="s">
-        <v>132</v>
+        <v>43</v>
+      </c>
+      <c r="AF88" t="s">
+        <v>122</v>
       </c>
       <c r="AG88">
-        <v>0.18181820000000001</v>
+        <v>1</v>
       </c>
       <c r="AH88" t="s">
         <v>56</v>
@@ -10276,7 +10311,7 @@
         <v>43</v>
       </c>
       <c r="AJ88">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="AK88">
         <v>1</v>
@@ -10293,10 +10328,10 @@
     </row>
     <row r="89" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B89" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C89" t="s">
         <v>43</v>
@@ -10329,19 +10364,19 @@
         <v>47</v>
       </c>
       <c r="M89" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N89">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O89">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P89">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q89">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R89" t="s">
         <v>49</v>
@@ -10356,13 +10391,13 @@
         <v>52</v>
       </c>
       <c r="V89" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="AA89" t="s">
         <v>54</v>
       </c>
       <c r="AB89">
-        <v>118831</v>
+        <v>109216</v>
       </c>
       <c r="AC89" t="s">
         <v>55</v>
@@ -10371,7 +10406,7 @@
         <v>43</v>
       </c>
       <c r="AG89">
-        <v>9.0909089999999998E-2</v>
+        <v>0.25</v>
       </c>
       <c r="AH89" t="s">
         <v>56</v>
@@ -10380,7 +10415,7 @@
         <v>43</v>
       </c>
       <c r="AJ89">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK89">
         <v>1</v>
@@ -10397,10 +10432,10 @@
     </row>
     <row r="90" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C90" t="s">
         <v>43</v>
@@ -10433,19 +10468,19 @@
         <v>47</v>
       </c>
       <c r="M90" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N90">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O90">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P90">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q90">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R90" t="s">
         <v>49</v>
@@ -10460,19 +10495,13 @@
         <v>52</v>
       </c>
       <c r="V90" t="s">
-        <v>61</v>
-      </c>
-      <c r="W90" t="s">
-        <v>116</v>
-      </c>
-      <c r="X90" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="AA90" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB90">
-        <v>109191</v>
+        <v>118831</v>
       </c>
       <c r="AC90" t="s">
         <v>55</v>
@@ -10481,7 +10510,7 @@
         <v>43</v>
       </c>
       <c r="AG90">
-        <v>9.0909089999999998E-2</v>
+        <v>0.125</v>
       </c>
       <c r="AH90" t="s">
         <v>56</v>
@@ -10490,7 +10519,7 @@
         <v>43</v>
       </c>
       <c r="AJ90">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK90">
         <v>1</v>
@@ -10507,10 +10536,10 @@
     </row>
     <row r="91" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C91" t="s">
         <v>43</v>
@@ -10543,19 +10572,19 @@
         <v>47</v>
       </c>
       <c r="M91" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N91">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O91">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P91">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q91">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R91" t="s">
         <v>49</v>
@@ -10578,17 +10607,11 @@
       <c r="X91" t="s">
         <v>133</v>
       </c>
-      <c r="Y91" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z91" t="s">
-        <v>135</v>
-      </c>
       <c r="AA91" t="s">
         <v>54</v>
       </c>
-      <c r="AB91">
-        <v>200660</v>
+      <c r="AB91" s="1">
+        <v>109191</v>
       </c>
       <c r="AC91" t="s">
         <v>55</v>
@@ -10596,8 +10619,11 @@
       <c r="AE91" t="s">
         <v>43</v>
       </c>
+      <c r="AF91" t="s">
+        <v>149</v>
+      </c>
       <c r="AG91">
-        <v>6.0606060000000003E-2</v>
+        <v>0.125</v>
       </c>
       <c r="AH91" t="s">
         <v>56</v>
@@ -10606,7 +10632,7 @@
         <v>43</v>
       </c>
       <c r="AJ91">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK91">
         <v>1</v>
@@ -10623,10 +10649,10 @@
     </row>
     <row r="92" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C92" t="s">
         <v>43</v>
@@ -10659,19 +10685,19 @@
         <v>47</v>
       </c>
       <c r="M92" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N92">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O92">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P92">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q92">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R92" t="s">
         <v>49</v>
@@ -10686,16 +10712,13 @@
         <v>52</v>
       </c>
       <c r="V92" t="s">
-        <v>61</v>
-      </c>
-      <c r="W92" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA92" t="s">
         <v>54</v>
       </c>
       <c r="AB92">
-        <v>103358</v>
+        <v>152741</v>
       </c>
       <c r="AC92" t="s">
         <v>55</v>
@@ -10704,7 +10727,7 @@
         <v>43</v>
       </c>
       <c r="AG92">
-        <v>9.0909089999999998E-2</v>
+        <v>0.125</v>
       </c>
       <c r="AH92" t="s">
         <v>56</v>
@@ -10713,7 +10736,7 @@
         <v>43</v>
       </c>
       <c r="AJ92">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK92">
         <v>1</v>
@@ -10730,10 +10753,10 @@
     </row>
     <row r="93" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C93" t="s">
         <v>43</v>
@@ -10766,19 +10789,19 @@
         <v>47</v>
       </c>
       <c r="M93" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N93">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O93">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P93">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q93">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R93" t="s">
         <v>49</v>
@@ -10793,22 +10816,25 @@
         <v>52</v>
       </c>
       <c r="V93" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AA93" t="s">
         <v>54</v>
       </c>
       <c r="AB93">
-        <v>152741</v>
+        <v>117232</v>
       </c>
       <c r="AC93" t="s">
         <v>55</v>
       </c>
+      <c r="AD93" t="s">
+        <v>67</v>
+      </c>
       <c r="AE93" t="s">
         <v>43</v>
       </c>
       <c r="AG93">
-        <v>6.0606060000000003E-2</v>
+        <v>0.125</v>
       </c>
       <c r="AH93" t="s">
         <v>56</v>
@@ -10817,13 +10843,16 @@
         <v>43</v>
       </c>
       <c r="AJ93">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK93">
         <v>1</v>
       </c>
       <c r="AL93" t="s">
         <v>57</v>
+      </c>
+      <c r="AM93" t="s">
+        <v>99</v>
       </c>
       <c r="AN93" t="s">
         <v>58</v>
@@ -10834,10 +10863,10 @@
     </row>
     <row r="94" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C94" t="s">
         <v>43</v>
@@ -10870,19 +10899,19 @@
         <v>47</v>
       </c>
       <c r="M94" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N94">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O94">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P94">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q94">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R94" t="s">
         <v>49</v>
@@ -10897,43 +10926,37 @@
         <v>52</v>
       </c>
       <c r="V94" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AA94" t="s">
         <v>54</v>
       </c>
       <c r="AB94">
-        <v>117232</v>
+        <v>109216</v>
       </c>
       <c r="AC94" t="s">
         <v>55</v>
       </c>
-      <c r="AD94" t="s">
-        <v>65</v>
-      </c>
       <c r="AE94" t="s">
         <v>43</v>
       </c>
       <c r="AG94">
-        <v>0.21212120000000001</v>
+        <v>0.48148148148148145</v>
       </c>
       <c r="AH94" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI94" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI94">
+        <v>27</v>
       </c>
       <c r="AJ94">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK94">
         <v>1</v>
       </c>
       <c r="AL94" t="s">
         <v>57</v>
-      </c>
-      <c r="AM94" t="s">
-        <v>99</v>
       </c>
       <c r="AN94" t="s">
         <v>58</v>
@@ -10944,10 +10967,10 @@
     </row>
     <row r="95" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B95" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C95" t="s">
         <v>43</v>
@@ -10980,19 +11003,19 @@
         <v>47</v>
       </c>
       <c r="M95" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N95">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O95">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P95">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q95">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R95" t="s">
         <v>49</v>
@@ -11006,32 +11029,32 @@
       <c r="U95" t="s">
         <v>52</v>
       </c>
+      <c r="V95" t="s">
+        <v>60</v>
+      </c>
       <c r="AA95" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB95">
-        <v>99208</v>
+        <v>118831</v>
       </c>
       <c r="AC95" t="s">
         <v>55</v>
       </c>
-      <c r="AD95" t="s">
-        <v>136</v>
-      </c>
       <c r="AE95" t="s">
         <v>43</v>
       </c>
       <c r="AG95">
-        <v>3.0303030000000002E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="AH95" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI95" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI95">
+        <v>27</v>
       </c>
       <c r="AJ95">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK95">
         <v>1</v>
@@ -11048,10 +11071,10 @@
     </row>
     <row r="96" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C96" t="s">
         <v>43</v>
@@ -11084,19 +11107,19 @@
         <v>47</v>
       </c>
       <c r="M96" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N96">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O96">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P96">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q96">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R96" t="s">
         <v>49</v>
@@ -11111,31 +11134,40 @@
         <v>52</v>
       </c>
       <c r="V96" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="W96" t="s">
+        <v>116</v>
+      </c>
+      <c r="X96" t="s">
+        <v>133</v>
       </c>
       <c r="AA96" t="s">
         <v>54</v>
       </c>
-      <c r="AB96">
-        <v>109216</v>
+      <c r="AB96" s="1">
+        <v>109191</v>
       </c>
       <c r="AC96" t="s">
         <v>55</v>
       </c>
       <c r="AE96" t="s">
-        <v>132</v>
+        <v>43</v>
+      </c>
+      <c r="AF96" t="s">
+        <v>149</v>
       </c>
       <c r="AG96">
-        <v>0.10833333333333334</v>
+        <v>0.18518518518518517</v>
       </c>
       <c r="AH96" t="s">
         <v>90</v>
       </c>
       <c r="AI96">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="AJ96">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK96">
         <v>1</v>
@@ -11144,7 +11176,7 @@
         <v>57</v>
       </c>
       <c r="AN96" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO96" t="s">
         <v>59</v>
@@ -11152,10 +11184,10 @@
     </row>
     <row r="97" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C97" t="s">
         <v>43</v>
@@ -11188,19 +11220,19 @@
         <v>47</v>
       </c>
       <c r="M97" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N97">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O97">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P97">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q97">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R97" t="s">
         <v>49</v>
@@ -11215,13 +11247,13 @@
         <v>52</v>
       </c>
       <c r="V97" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AA97" t="s">
         <v>54</v>
       </c>
       <c r="AB97">
-        <v>118831</v>
+        <v>152741</v>
       </c>
       <c r="AC97" t="s">
         <v>55</v>
@@ -11230,16 +11262,16 @@
         <v>43</v>
       </c>
       <c r="AG97">
-        <v>0.125</v>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="AH97" t="s">
         <v>90</v>
       </c>
       <c r="AI97">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="AJ97">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK97">
         <v>1</v>
@@ -11248,7 +11280,7 @@
         <v>57</v>
       </c>
       <c r="AN97" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO97" t="s">
         <v>59</v>
@@ -11256,10 +11288,10 @@
     </row>
     <row r="98" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C98" t="s">
         <v>43</v>
@@ -11292,19 +11324,19 @@
         <v>47</v>
       </c>
       <c r="M98" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N98">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O98">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P98">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q98">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R98" t="s">
         <v>49</v>
@@ -11319,37 +11351,34 @@
         <v>52</v>
       </c>
       <c r="V98" t="s">
-        <v>61</v>
-      </c>
-      <c r="W98" t="s">
-        <v>116</v>
-      </c>
-      <c r="X98" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="AA98" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB98">
-        <v>109191</v>
+        <v>117232</v>
       </c>
       <c r="AC98" t="s">
         <v>55</v>
       </c>
+      <c r="AD98" t="s">
+        <v>67</v>
+      </c>
       <c r="AE98" t="s">
         <v>43</v>
       </c>
       <c r="AG98">
-        <v>0.33333333333333331</v>
+        <v>0.18518518518518517</v>
       </c>
       <c r="AH98" t="s">
         <v>90</v>
       </c>
       <c r="AI98">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="AJ98">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AK98">
         <v>1</v>
@@ -11357,8 +11386,11 @@
       <c r="AL98" t="s">
         <v>57</v>
       </c>
+      <c r="AM98" t="s">
+        <v>99</v>
+      </c>
       <c r="AN98" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO98" t="s">
         <v>59</v>
@@ -11366,10 +11398,10 @@
     </row>
     <row r="99" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C99" t="s">
         <v>43</v>
@@ -11399,25 +11431,25 @@
         <v>46</v>
       </c>
       <c r="L99" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
       <c r="M99" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N99">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O99">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P99">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q99">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R99" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="S99" t="s">
         <v>50</v>
@@ -11431,23 +11463,11 @@
       <c r="V99" t="s">
         <v>61</v>
       </c>
-      <c r="W99" t="s">
-        <v>116</v>
-      </c>
-      <c r="X99" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y99" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z99" t="s">
-        <v>135</v>
-      </c>
       <c r="AA99" t="s">
         <v>54</v>
       </c>
       <c r="AB99">
-        <v>200660</v>
+        <v>103359</v>
       </c>
       <c r="AC99" t="s">
         <v>55</v>
@@ -11456,16 +11476,16 @@
         <v>43</v>
       </c>
       <c r="AG99">
-        <v>1.6666666666666666E-2</v>
+        <v>1</v>
       </c>
       <c r="AH99" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI99">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI99" t="s">
+        <v>43</v>
       </c>
       <c r="AJ99">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="AK99">
         <v>1</v>
@@ -11474,7 +11494,7 @@
         <v>57</v>
       </c>
       <c r="AN99" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO99" t="s">
         <v>59</v>
@@ -11482,10 +11502,10 @@
     </row>
     <row r="100" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B100" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C100" t="s">
         <v>43</v>
@@ -11515,46 +11535,34 @@
         <v>46</v>
       </c>
       <c r="L100" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
       <c r="M100" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="N100">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O100">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="P100">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q100">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="R100" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="S100" t="s">
-        <v>50</v>
-      </c>
-      <c r="T100" t="s">
-        <v>51</v>
-      </c>
-      <c r="U100" t="s">
-        <v>52</v>
-      </c>
-      <c r="V100" t="s">
-        <v>61</v>
-      </c>
-      <c r="W100" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="AA100" t="s">
         <v>54</v>
       </c>
       <c r="AB100">
-        <v>103358</v>
+        <v>202422</v>
       </c>
       <c r="AC100" t="s">
         <v>55</v>
@@ -11562,17 +11570,20 @@
       <c r="AE100" t="s">
         <v>43</v>
       </c>
+      <c r="AF100" t="s">
+        <v>129</v>
+      </c>
       <c r="AG100">
-        <v>0.29166666666666669</v>
+        <v>1</v>
       </c>
       <c r="AH100" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI100">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI100" t="s">
+        <v>43</v>
       </c>
       <c r="AJ100">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="AK100">
         <v>1</v>
@@ -11581,7 +11592,7 @@
         <v>57</v>
       </c>
       <c r="AN100" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO100" t="s">
         <v>59</v>
@@ -11652,28 +11663,28 @@
         <v>52</v>
       </c>
       <c r="V101" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="AA101" t="s">
         <v>54</v>
       </c>
       <c r="AB101">
-        <v>152741</v>
+        <v>109216</v>
       </c>
       <c r="AC101" t="s">
         <v>55</v>
       </c>
       <c r="AE101" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="AG101">
-        <v>1.6666666666666666E-2</v>
+        <v>0.18181820000000001</v>
       </c>
       <c r="AH101" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI101">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI101" t="s">
+        <v>43</v>
       </c>
       <c r="AJ101">
         <v>33</v>
@@ -11685,7 +11696,7 @@
         <v>57</v>
       </c>
       <c r="AN101" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO101" t="s">
         <v>59</v>
@@ -11756,31 +11767,28 @@
         <v>52</v>
       </c>
       <c r="V102" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AA102" t="s">
         <v>54</v>
       </c>
       <c r="AB102">
-        <v>117232</v>
+        <v>118831</v>
       </c>
       <c r="AC102" t="s">
         <v>55</v>
       </c>
-      <c r="AD102" t="s">
-        <v>65</v>
-      </c>
       <c r="AE102" t="s">
         <v>43</v>
       </c>
       <c r="AG102">
-        <v>0.10833333333333334</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH102" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI102">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI102" t="s">
+        <v>43</v>
       </c>
       <c r="AJ102">
         <v>33</v>
@@ -11791,11 +11799,8 @@
       <c r="AL102" t="s">
         <v>57</v>
       </c>
-      <c r="AM102" t="s">
-        <v>99</v>
-      </c>
       <c r="AN102" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO102" t="s">
         <v>59</v>
@@ -11865,29 +11870,35 @@
       <c r="U103" t="s">
         <v>52</v>
       </c>
+      <c r="V103" t="s">
+        <v>61</v>
+      </c>
+      <c r="W103" t="s">
+        <v>116</v>
+      </c>
+      <c r="X103" t="s">
+        <v>133</v>
+      </c>
       <c r="AA103" t="s">
         <v>94</v>
       </c>
       <c r="AB103">
-        <v>99208</v>
+        <v>109191</v>
       </c>
       <c r="AC103" t="s">
         <v>55</v>
       </c>
-      <c r="AD103" t="s">
-        <v>136</v>
-      </c>
       <c r="AE103" t="s">
         <v>43</v>
       </c>
       <c r="AG103">
-        <v>9.1666999999999998E-2</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH103" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI103">
-        <v>131</v>
+        <v>56</v>
+      </c>
+      <c r="AI103" t="s">
+        <v>43</v>
       </c>
       <c r="AJ103">
         <v>33</v>
@@ -11899,7 +11910,7 @@
         <v>57</v>
       </c>
       <c r="AN103" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="AO103" t="s">
         <v>59</v>
@@ -11907,13 +11918,13 @@
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C104" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D104" t="s">
         <v>44</v>
@@ -11940,22 +11951,22 @@
         <v>46</v>
       </c>
       <c r="L104" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M104" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N104">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O104">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P104">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q104">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R104" t="s">
         <v>49</v>
@@ -11967,16 +11978,28 @@
         <v>51</v>
       </c>
       <c r="U104" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="V104" t="s">
-        <v>142</v>
+        <v>61</v>
+      </c>
+      <c r="W104" t="s">
+        <v>116</v>
+      </c>
+      <c r="X104" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y104" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z104" t="s">
+        <v>135</v>
       </c>
       <c r="AA104" t="s">
         <v>54</v>
       </c>
       <c r="AB104">
-        <v>82732</v>
+        <v>200660</v>
       </c>
       <c r="AC104" t="s">
         <v>55</v>
@@ -11985,7 +12008,7 @@
         <v>43</v>
       </c>
       <c r="AG104">
-        <v>4.7619050000000003E-2</v>
+        <v>6.0606060000000003E-2</v>
       </c>
       <c r="AH104" t="s">
         <v>56</v>
@@ -11994,7 +12017,7 @@
         <v>43</v>
       </c>
       <c r="AJ104">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK104">
         <v>1</v>
@@ -12011,13 +12034,13 @@
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B105" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C105" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D105" t="s">
         <v>44</v>
@@ -12044,22 +12067,22 @@
         <v>46</v>
       </c>
       <c r="L105" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M105" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N105">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O105">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P105">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q105">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R105" t="s">
         <v>49</v>
@@ -12074,13 +12097,16 @@
         <v>52</v>
       </c>
       <c r="V105" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="W105" t="s">
+        <v>62</v>
       </c>
       <c r="AA105" t="s">
         <v>54</v>
       </c>
       <c r="AB105">
-        <v>109216</v>
+        <v>103358</v>
       </c>
       <c r="AC105" t="s">
         <v>55</v>
@@ -12089,7 +12115,7 @@
         <v>43</v>
       </c>
       <c r="AG105">
-        <v>0.71428570000000002</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="AH105" t="s">
         <v>56</v>
@@ -12098,7 +12124,7 @@
         <v>43</v>
       </c>
       <c r="AJ105">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK105">
         <v>1</v>
@@ -12115,13 +12141,13 @@
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B106" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C106" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D106" t="s">
         <v>44</v>
@@ -12148,22 +12174,22 @@
         <v>46</v>
       </c>
       <c r="L106" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M106" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N106">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O106">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P106">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q106">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R106" t="s">
         <v>49</v>
@@ -12178,13 +12204,13 @@
         <v>52</v>
       </c>
       <c r="V106" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AA106" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB106">
-        <v>118831</v>
+        <v>152741</v>
       </c>
       <c r="AC106" t="s">
         <v>55</v>
@@ -12193,7 +12219,7 @@
         <v>43</v>
       </c>
       <c r="AG106">
-        <v>0.23809520000000001</v>
+        <v>6.0606060000000003E-2</v>
       </c>
       <c r="AH106" t="s">
         <v>56</v>
@@ -12202,7 +12228,7 @@
         <v>43</v>
       </c>
       <c r="AJ106">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK106">
         <v>1</v>
@@ -12219,13 +12245,13 @@
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B107" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C107" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D107" t="s">
         <v>44</v>
@@ -12252,22 +12278,22 @@
         <v>46</v>
       </c>
       <c r="L107" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M107" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N107">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O107">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P107">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q107">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R107" t="s">
         <v>49</v>
@@ -12282,31 +12308,25 @@
         <v>52</v>
       </c>
       <c r="V107" t="s">
-        <v>60</v>
-      </c>
-      <c r="W107" t="s">
-        <v>105</v>
-      </c>
-      <c r="X107" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="AA107" t="s">
         <v>54</v>
       </c>
       <c r="AB107">
-        <v>118840</v>
+        <v>117232</v>
       </c>
       <c r="AC107" t="s">
         <v>55</v>
       </c>
       <c r="AD107" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="AE107" t="s">
         <v>43</v>
       </c>
       <c r="AG107">
-        <v>4.7619050000000003E-2</v>
+        <v>0.21212120000000001</v>
       </c>
       <c r="AH107" t="s">
         <v>56</v>
@@ -12315,13 +12335,16 @@
         <v>43</v>
       </c>
       <c r="AJ107">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK107">
         <v>1</v>
       </c>
       <c r="AL107" t="s">
         <v>57</v>
+      </c>
+      <c r="AM107" t="s">
+        <v>99</v>
       </c>
       <c r="AN107" t="s">
         <v>58</v>
@@ -12332,13 +12355,13 @@
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B108" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C108" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D108" t="s">
         <v>44</v>
@@ -12365,22 +12388,22 @@
         <v>46</v>
       </c>
       <c r="L108" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M108" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N108">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O108">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P108">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q108">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R108" t="s">
         <v>49</v>
@@ -12394,29 +12417,23 @@
       <c r="U108" t="s">
         <v>52</v>
       </c>
-      <c r="V108" t="s">
-        <v>63</v>
-      </c>
-      <c r="W108" t="s">
-        <v>96</v>
-      </c>
-      <c r="X108" t="s">
-        <v>98</v>
-      </c>
       <c r="AA108" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB108">
-        <v>153360</v>
+        <v>99208</v>
       </c>
       <c r="AC108" t="s">
         <v>55</v>
       </c>
+      <c r="AD108" t="s">
+        <v>136</v>
+      </c>
       <c r="AE108" t="s">
         <v>43</v>
       </c>
       <c r="AG108">
-        <v>4.7619050000000003E-2</v>
+        <v>3.0303030000000002E-2</v>
       </c>
       <c r="AH108" t="s">
         <v>56</v>
@@ -12425,7 +12442,7 @@
         <v>43</v>
       </c>
       <c r="AJ108">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK108">
         <v>1</v>
@@ -12442,13 +12459,13 @@
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B109" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C109" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D109" t="s">
         <v>44</v>
@@ -12475,22 +12492,22 @@
         <v>46</v>
       </c>
       <c r="L109" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M109" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N109">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O109">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P109">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q109">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R109" t="s">
         <v>49</v>
@@ -12505,37 +12522,31 @@
         <v>52</v>
       </c>
       <c r="V109" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AA109" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="AB109">
-        <v>117232</v>
+        <v>109216</v>
       </c>
       <c r="AC109" t="s">
         <v>55</v>
       </c>
-      <c r="AD109" t="s">
-        <v>67</v>
-      </c>
       <c r="AE109" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF109" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="AG109">
-        <v>4.7619050000000003E-2</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="AH109" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI109" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI109">
+        <v>131</v>
       </c>
       <c r="AJ109">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK109">
         <v>1</v>
@@ -12544,7 +12555,7 @@
         <v>57</v>
       </c>
       <c r="AN109" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="AO109" t="s">
         <v>59</v>
@@ -12552,13 +12563,13 @@
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C110" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D110" t="s">
         <v>44</v>
@@ -12585,22 +12596,22 @@
         <v>46</v>
       </c>
       <c r="L110" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M110" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N110">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O110">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P110">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q110">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R110" t="s">
         <v>49</v>
@@ -12615,43 +12626,31 @@
         <v>52</v>
       </c>
       <c r="V110" t="s">
-        <v>64</v>
-      </c>
-      <c r="X110" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y110" t="s">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="AA110" t="s">
         <v>54</v>
       </c>
       <c r="AB110">
-        <v>117478</v>
+        <v>118831</v>
       </c>
       <c r="AC110" t="s">
         <v>55</v>
       </c>
-      <c r="AD110" t="s">
-        <v>65</v>
-      </c>
       <c r="AE110" t="s">
         <v>43</v>
       </c>
-      <c r="AF110" t="s">
-        <v>145</v>
-      </c>
       <c r="AG110">
-        <v>9.5238089999999997E-2</v>
+        <v>0.125</v>
       </c>
       <c r="AH110" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI110" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI110">
+        <v>131</v>
       </c>
       <c r="AJ110">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK110">
         <v>1</v>
@@ -12660,7 +12659,7 @@
         <v>57</v>
       </c>
       <c r="AN110" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="AO110" t="s">
         <v>59</v>
@@ -12668,13 +12667,13 @@
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B111" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C111" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D111" t="s">
         <v>44</v>
@@ -12701,22 +12700,22 @@
         <v>46</v>
       </c>
       <c r="L111" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="M111" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="N111">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O111">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="P111">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q111">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="R111" t="s">
         <v>49</v>
@@ -12731,13 +12730,19 @@
         <v>52</v>
       </c>
       <c r="V111" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="W111" t="s">
+        <v>116</v>
+      </c>
+      <c r="X111" t="s">
+        <v>133</v>
       </c>
       <c r="AA111" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="AB111">
-        <v>115095</v>
+        <v>109191</v>
       </c>
       <c r="AC111" t="s">
         <v>55</v>
@@ -12746,16 +12751,16 @@
         <v>43</v>
       </c>
       <c r="AG111">
-        <v>4.7619050000000003E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AH111" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI111" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="AI111">
+        <v>131</v>
       </c>
       <c r="AJ111">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AK111">
         <v>1</v>
@@ -12764,9 +12769,1415 @@
         <v>57</v>
       </c>
       <c r="AN111" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO111" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>130</v>
+      </c>
+      <c r="B112" t="s">
+        <v>131</v>
+      </c>
+      <c r="C112" t="s">
+        <v>43</v>
+      </c>
+      <c r="D112" t="s">
+        <v>44</v>
+      </c>
+      <c r="E112" t="s">
+        <v>45</v>
+      </c>
+      <c r="F112" t="s">
+        <v>43</v>
+      </c>
+      <c r="G112" t="s">
+        <v>43</v>
+      </c>
+      <c r="H112" t="s">
+        <v>43</v>
+      </c>
+      <c r="I112" t="s">
+        <v>43</v>
+      </c>
+      <c r="J112" t="s">
+        <v>43</v>
+      </c>
+      <c r="K112" t="s">
+        <v>46</v>
+      </c>
+      <c r="L112" t="s">
+        <v>47</v>
+      </c>
+      <c r="M112" t="s">
+        <v>72</v>
+      </c>
+      <c r="N112">
+        <v>9</v>
+      </c>
+      <c r="O112">
+        <v>1877</v>
+      </c>
+      <c r="P112">
+        <v>9</v>
+      </c>
+      <c r="Q112">
+        <v>1877</v>
+      </c>
+      <c r="R112" t="s">
+        <v>49</v>
+      </c>
+      <c r="S112" t="s">
+        <v>50</v>
+      </c>
+      <c r="T112" t="s">
+        <v>51</v>
+      </c>
+      <c r="U112" t="s">
+        <v>52</v>
+      </c>
+      <c r="V112" t="s">
+        <v>61</v>
+      </c>
+      <c r="W112" t="s">
+        <v>116</v>
+      </c>
+      <c r="X112" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y112" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z112" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA112" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB112">
+        <v>200660</v>
+      </c>
+      <c r="AC112" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE112" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG112">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="AH112" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI112">
+        <v>131</v>
+      </c>
+      <c r="AJ112">
+        <v>33</v>
+      </c>
+      <c r="AK112">
+        <v>1</v>
+      </c>
+      <c r="AL112" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN112" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO112" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>130</v>
+      </c>
+      <c r="B113" t="s">
+        <v>131</v>
+      </c>
+      <c r="C113" t="s">
+        <v>43</v>
+      </c>
+      <c r="D113" t="s">
+        <v>44</v>
+      </c>
+      <c r="E113" t="s">
+        <v>45</v>
+      </c>
+      <c r="F113" t="s">
+        <v>43</v>
+      </c>
+      <c r="G113" t="s">
+        <v>43</v>
+      </c>
+      <c r="H113" t="s">
+        <v>43</v>
+      </c>
+      <c r="I113" t="s">
+        <v>43</v>
+      </c>
+      <c r="J113" t="s">
+        <v>43</v>
+      </c>
+      <c r="K113" t="s">
+        <v>46</v>
+      </c>
+      <c r="L113" t="s">
+        <v>47</v>
+      </c>
+      <c r="M113" t="s">
+        <v>72</v>
+      </c>
+      <c r="N113">
+        <v>9</v>
+      </c>
+      <c r="O113">
+        <v>1877</v>
+      </c>
+      <c r="P113">
+        <v>9</v>
+      </c>
+      <c r="Q113">
+        <v>1877</v>
+      </c>
+      <c r="R113" t="s">
+        <v>49</v>
+      </c>
+      <c r="S113" t="s">
+        <v>50</v>
+      </c>
+      <c r="T113" t="s">
+        <v>51</v>
+      </c>
+      <c r="U113" t="s">
+        <v>52</v>
+      </c>
+      <c r="V113" t="s">
+        <v>61</v>
+      </c>
+      <c r="W113" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA113" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB113">
+        <v>103358</v>
+      </c>
+      <c r="AC113" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE113" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG113">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="AH113" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI113">
+        <v>131</v>
+      </c>
+      <c r="AJ113">
+        <v>33</v>
+      </c>
+      <c r="AK113">
+        <v>1</v>
+      </c>
+      <c r="AL113" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN113" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO113" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>130</v>
+      </c>
+      <c r="B114" t="s">
+        <v>131</v>
+      </c>
+      <c r="C114" t="s">
+        <v>43</v>
+      </c>
+      <c r="D114" t="s">
+        <v>44</v>
+      </c>
+      <c r="E114" t="s">
+        <v>45</v>
+      </c>
+      <c r="F114" t="s">
+        <v>43</v>
+      </c>
+      <c r="G114" t="s">
+        <v>43</v>
+      </c>
+      <c r="H114" t="s">
+        <v>43</v>
+      </c>
+      <c r="I114" t="s">
+        <v>43</v>
+      </c>
+      <c r="J114" t="s">
+        <v>43</v>
+      </c>
+      <c r="K114" t="s">
+        <v>46</v>
+      </c>
+      <c r="L114" t="s">
+        <v>47</v>
+      </c>
+      <c r="M114" t="s">
+        <v>72</v>
+      </c>
+      <c r="N114">
+        <v>9</v>
+      </c>
+      <c r="O114">
+        <v>1877</v>
+      </c>
+      <c r="P114">
+        <v>9</v>
+      </c>
+      <c r="Q114">
+        <v>1877</v>
+      </c>
+      <c r="R114" t="s">
+        <v>49</v>
+      </c>
+      <c r="S114" t="s">
+        <v>50</v>
+      </c>
+      <c r="T114" t="s">
+        <v>51</v>
+      </c>
+      <c r="U114" t="s">
+        <v>52</v>
+      </c>
+      <c r="V114" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA114" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB114">
+        <v>152741</v>
+      </c>
+      <c r="AC114" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE114" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG114">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="AH114" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI114">
+        <v>131</v>
+      </c>
+      <c r="AJ114">
+        <v>33</v>
+      </c>
+      <c r="AK114">
+        <v>1</v>
+      </c>
+      <c r="AL114" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN114" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO114" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>130</v>
+      </c>
+      <c r="B115" t="s">
+        <v>131</v>
+      </c>
+      <c r="C115" t="s">
+        <v>43</v>
+      </c>
+      <c r="D115" t="s">
+        <v>44</v>
+      </c>
+      <c r="E115" t="s">
+        <v>45</v>
+      </c>
+      <c r="F115" t="s">
+        <v>43</v>
+      </c>
+      <c r="G115" t="s">
+        <v>43</v>
+      </c>
+      <c r="H115" t="s">
+        <v>43</v>
+      </c>
+      <c r="I115" t="s">
+        <v>43</v>
+      </c>
+      <c r="J115" t="s">
+        <v>43</v>
+      </c>
+      <c r="K115" t="s">
+        <v>46</v>
+      </c>
+      <c r="L115" t="s">
+        <v>47</v>
+      </c>
+      <c r="M115" t="s">
+        <v>72</v>
+      </c>
+      <c r="N115">
+        <v>9</v>
+      </c>
+      <c r="O115">
+        <v>1877</v>
+      </c>
+      <c r="P115">
+        <v>9</v>
+      </c>
+      <c r="Q115">
+        <v>1877</v>
+      </c>
+      <c r="R115" t="s">
+        <v>49</v>
+      </c>
+      <c r="S115" t="s">
+        <v>50</v>
+      </c>
+      <c r="T115" t="s">
+        <v>51</v>
+      </c>
+      <c r="U115" t="s">
+        <v>52</v>
+      </c>
+      <c r="V115" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA115" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB115">
+        <v>117232</v>
+      </c>
+      <c r="AC115" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD115" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE115" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG115">
+        <v>0.10833333333333334</v>
+      </c>
+      <c r="AH115" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI115">
+        <v>131</v>
+      </c>
+      <c r="AJ115">
+        <v>33</v>
+      </c>
+      <c r="AK115">
+        <v>1</v>
+      </c>
+      <c r="AL115" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM115" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN115" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO115" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>130</v>
+      </c>
+      <c r="B116" t="s">
+        <v>131</v>
+      </c>
+      <c r="C116" t="s">
+        <v>43</v>
+      </c>
+      <c r="D116" t="s">
+        <v>44</v>
+      </c>
+      <c r="E116" t="s">
+        <v>45</v>
+      </c>
+      <c r="F116" t="s">
+        <v>43</v>
+      </c>
+      <c r="G116" t="s">
+        <v>43</v>
+      </c>
+      <c r="H116" t="s">
+        <v>43</v>
+      </c>
+      <c r="I116" t="s">
+        <v>43</v>
+      </c>
+      <c r="J116" t="s">
+        <v>43</v>
+      </c>
+      <c r="K116" t="s">
+        <v>46</v>
+      </c>
+      <c r="L116" t="s">
+        <v>47</v>
+      </c>
+      <c r="M116" t="s">
+        <v>72</v>
+      </c>
+      <c r="N116">
+        <v>9</v>
+      </c>
+      <c r="O116">
+        <v>1877</v>
+      </c>
+      <c r="P116">
+        <v>9</v>
+      </c>
+      <c r="Q116">
+        <v>1877</v>
+      </c>
+      <c r="R116" t="s">
+        <v>49</v>
+      </c>
+      <c r="S116" t="s">
+        <v>50</v>
+      </c>
+      <c r="T116" t="s">
+        <v>51</v>
+      </c>
+      <c r="U116" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA116" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB116">
+        <v>99208</v>
+      </c>
+      <c r="AC116" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD116" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE116" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG116">
+        <v>9.1666999999999998E-2</v>
+      </c>
+      <c r="AH116" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI116">
+        <v>131</v>
+      </c>
+      <c r="AJ116">
+        <v>33</v>
+      </c>
+      <c r="AK116">
+        <v>1</v>
+      </c>
+      <c r="AL116" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN116" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>137</v>
+      </c>
+      <c r="B117" t="s">
+        <v>138</v>
+      </c>
+      <c r="C117" t="s">
+        <v>139</v>
+      </c>
+      <c r="D117" t="s">
+        <v>44</v>
+      </c>
+      <c r="E117" t="s">
+        <v>45</v>
+      </c>
+      <c r="F117" t="s">
+        <v>43</v>
+      </c>
+      <c r="G117" t="s">
+        <v>43</v>
+      </c>
+      <c r="H117" t="s">
+        <v>43</v>
+      </c>
+      <c r="I117" t="s">
+        <v>43</v>
+      </c>
+      <c r="J117" t="s">
+        <v>43</v>
+      </c>
+      <c r="K117" t="s">
+        <v>46</v>
+      </c>
+      <c r="L117" t="s">
+        <v>140</v>
+      </c>
+      <c r="M117" t="s">
+        <v>141</v>
+      </c>
+      <c r="N117">
+        <v>7</v>
+      </c>
+      <c r="O117">
+        <v>1876</v>
+      </c>
+      <c r="P117">
+        <v>7</v>
+      </c>
+      <c r="Q117">
+        <v>1876</v>
+      </c>
+      <c r="R117" t="s">
+        <v>49</v>
+      </c>
+      <c r="S117" t="s">
+        <v>50</v>
+      </c>
+      <c r="T117" t="s">
+        <v>51</v>
+      </c>
+      <c r="U117" t="s">
+        <v>102</v>
+      </c>
+      <c r="V117" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA117" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB117">
+        <v>82732</v>
+      </c>
+      <c r="AC117" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE117" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG117">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH117" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI117" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ117">
+        <v>21</v>
+      </c>
+      <c r="AK117">
+        <v>1</v>
+      </c>
+      <c r="AL117" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN117" t="s">
         <v>58</v>
       </c>
-      <c r="AO111" t="s">
+      <c r="AO117" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>137</v>
+      </c>
+      <c r="B118" t="s">
+        <v>138</v>
+      </c>
+      <c r="C118" t="s">
+        <v>139</v>
+      </c>
+      <c r="D118" t="s">
+        <v>44</v>
+      </c>
+      <c r="E118" t="s">
+        <v>45</v>
+      </c>
+      <c r="F118" t="s">
+        <v>43</v>
+      </c>
+      <c r="G118" t="s">
+        <v>43</v>
+      </c>
+      <c r="H118" t="s">
+        <v>43</v>
+      </c>
+      <c r="I118" t="s">
+        <v>43</v>
+      </c>
+      <c r="J118" t="s">
+        <v>43</v>
+      </c>
+      <c r="K118" t="s">
+        <v>46</v>
+      </c>
+      <c r="L118" t="s">
+        <v>140</v>
+      </c>
+      <c r="M118" t="s">
+        <v>141</v>
+      </c>
+      <c r="N118">
+        <v>7</v>
+      </c>
+      <c r="O118">
+        <v>1876</v>
+      </c>
+      <c r="P118">
+        <v>7</v>
+      </c>
+      <c r="Q118">
+        <v>1876</v>
+      </c>
+      <c r="R118" t="s">
+        <v>49</v>
+      </c>
+      <c r="S118" t="s">
+        <v>50</v>
+      </c>
+      <c r="T118" t="s">
+        <v>51</v>
+      </c>
+      <c r="U118" t="s">
+        <v>52</v>
+      </c>
+      <c r="V118" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA118" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB118">
+        <v>109216</v>
+      </c>
+      <c r="AC118" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE118" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG118">
+        <v>0.71428570000000002</v>
+      </c>
+      <c r="AH118" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI118" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ118">
+        <v>21</v>
+      </c>
+      <c r="AK118">
+        <v>1</v>
+      </c>
+      <c r="AL118" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN118" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO118" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>137</v>
+      </c>
+      <c r="B119" t="s">
+        <v>138</v>
+      </c>
+      <c r="C119" t="s">
+        <v>139</v>
+      </c>
+      <c r="D119" t="s">
+        <v>44</v>
+      </c>
+      <c r="E119" t="s">
+        <v>45</v>
+      </c>
+      <c r="F119" t="s">
+        <v>43</v>
+      </c>
+      <c r="G119" t="s">
+        <v>43</v>
+      </c>
+      <c r="H119" t="s">
+        <v>43</v>
+      </c>
+      <c r="I119" t="s">
+        <v>43</v>
+      </c>
+      <c r="J119" t="s">
+        <v>43</v>
+      </c>
+      <c r="K119" t="s">
+        <v>46</v>
+      </c>
+      <c r="L119" t="s">
+        <v>140</v>
+      </c>
+      <c r="M119" t="s">
+        <v>141</v>
+      </c>
+      <c r="N119">
+        <v>7</v>
+      </c>
+      <c r="O119">
+        <v>1876</v>
+      </c>
+      <c r="P119">
+        <v>7</v>
+      </c>
+      <c r="Q119">
+        <v>1876</v>
+      </c>
+      <c r="R119" t="s">
+        <v>49</v>
+      </c>
+      <c r="S119" t="s">
+        <v>50</v>
+      </c>
+      <c r="T119" t="s">
+        <v>51</v>
+      </c>
+      <c r="U119" t="s">
+        <v>52</v>
+      </c>
+      <c r="V119" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA119" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB119">
+        <v>118831</v>
+      </c>
+      <c r="AC119" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE119" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG119">
+        <v>0.23809520000000001</v>
+      </c>
+      <c r="AH119" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI119" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ119">
+        <v>21</v>
+      </c>
+      <c r="AK119">
+        <v>1</v>
+      </c>
+      <c r="AL119" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN119" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO119" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>137</v>
+      </c>
+      <c r="B120" t="s">
+        <v>138</v>
+      </c>
+      <c r="C120" t="s">
+        <v>139</v>
+      </c>
+      <c r="D120" t="s">
+        <v>44</v>
+      </c>
+      <c r="E120" t="s">
+        <v>45</v>
+      </c>
+      <c r="F120" t="s">
+        <v>43</v>
+      </c>
+      <c r="G120" t="s">
+        <v>43</v>
+      </c>
+      <c r="H120" t="s">
+        <v>43</v>
+      </c>
+      <c r="I120" t="s">
+        <v>43</v>
+      </c>
+      <c r="J120" t="s">
+        <v>43</v>
+      </c>
+      <c r="K120" t="s">
+        <v>46</v>
+      </c>
+      <c r="L120" t="s">
+        <v>140</v>
+      </c>
+      <c r="M120" t="s">
+        <v>141</v>
+      </c>
+      <c r="N120">
+        <v>7</v>
+      </c>
+      <c r="O120">
+        <v>1876</v>
+      </c>
+      <c r="P120">
+        <v>7</v>
+      </c>
+      <c r="Q120">
+        <v>1876</v>
+      </c>
+      <c r="R120" t="s">
+        <v>49</v>
+      </c>
+      <c r="S120" t="s">
+        <v>50</v>
+      </c>
+      <c r="T120" t="s">
+        <v>51</v>
+      </c>
+      <c r="U120" t="s">
+        <v>52</v>
+      </c>
+      <c r="V120" t="s">
+        <v>60</v>
+      </c>
+      <c r="W120" t="s">
+        <v>105</v>
+      </c>
+      <c r="X120" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA120" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB120">
+        <v>118840</v>
+      </c>
+      <c r="AC120" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD120" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE120" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG120">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH120" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI120" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ120">
+        <v>21</v>
+      </c>
+      <c r="AK120">
+        <v>1</v>
+      </c>
+      <c r="AL120" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN120" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO120" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>137</v>
+      </c>
+      <c r="B121" t="s">
+        <v>138</v>
+      </c>
+      <c r="C121" t="s">
+        <v>139</v>
+      </c>
+      <c r="D121" t="s">
+        <v>44</v>
+      </c>
+      <c r="E121" t="s">
+        <v>45</v>
+      </c>
+      <c r="F121" t="s">
+        <v>43</v>
+      </c>
+      <c r="G121" t="s">
+        <v>43</v>
+      </c>
+      <c r="H121" t="s">
+        <v>43</v>
+      </c>
+      <c r="I121" t="s">
+        <v>43</v>
+      </c>
+      <c r="J121" t="s">
+        <v>43</v>
+      </c>
+      <c r="K121" t="s">
+        <v>46</v>
+      </c>
+      <c r="L121" t="s">
+        <v>140</v>
+      </c>
+      <c r="M121" t="s">
+        <v>141</v>
+      </c>
+      <c r="N121">
+        <v>7</v>
+      </c>
+      <c r="O121">
+        <v>1876</v>
+      </c>
+      <c r="P121">
+        <v>7</v>
+      </c>
+      <c r="Q121">
+        <v>1876</v>
+      </c>
+      <c r="R121" t="s">
+        <v>49</v>
+      </c>
+      <c r="S121" t="s">
+        <v>50</v>
+      </c>
+      <c r="T121" t="s">
+        <v>51</v>
+      </c>
+      <c r="U121" t="s">
+        <v>52</v>
+      </c>
+      <c r="V121" t="s">
+        <v>63</v>
+      </c>
+      <c r="W121" t="s">
+        <v>96</v>
+      </c>
+      <c r="X121" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA121" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB121">
+        <v>153360</v>
+      </c>
+      <c r="AC121" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE121" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG121">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH121" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI121" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ121">
+        <v>21</v>
+      </c>
+      <c r="AK121">
+        <v>1</v>
+      </c>
+      <c r="AL121" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN121" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO121" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>137</v>
+      </c>
+      <c r="B122" t="s">
+        <v>138</v>
+      </c>
+      <c r="C122" t="s">
+        <v>139</v>
+      </c>
+      <c r="D122" t="s">
+        <v>44</v>
+      </c>
+      <c r="E122" t="s">
+        <v>45</v>
+      </c>
+      <c r="F122" t="s">
+        <v>43</v>
+      </c>
+      <c r="G122" t="s">
+        <v>43</v>
+      </c>
+      <c r="H122" t="s">
+        <v>43</v>
+      </c>
+      <c r="I122" t="s">
+        <v>43</v>
+      </c>
+      <c r="J122" t="s">
+        <v>43</v>
+      </c>
+      <c r="K122" t="s">
+        <v>46</v>
+      </c>
+      <c r="L122" t="s">
+        <v>140</v>
+      </c>
+      <c r="M122" t="s">
+        <v>141</v>
+      </c>
+      <c r="N122">
+        <v>7</v>
+      </c>
+      <c r="O122">
+        <v>1876</v>
+      </c>
+      <c r="P122">
+        <v>7</v>
+      </c>
+      <c r="Q122">
+        <v>1876</v>
+      </c>
+      <c r="R122" t="s">
+        <v>49</v>
+      </c>
+      <c r="S122" t="s">
+        <v>50</v>
+      </c>
+      <c r="T122" t="s">
+        <v>51</v>
+      </c>
+      <c r="U122" t="s">
+        <v>52</v>
+      </c>
+      <c r="V122" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA122" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB122">
+        <v>117232</v>
+      </c>
+      <c r="AC122" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD122" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE122" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF122" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG122">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH122" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI122" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ122">
+        <v>21</v>
+      </c>
+      <c r="AK122">
+        <v>1</v>
+      </c>
+      <c r="AL122" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN122" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO122" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>137</v>
+      </c>
+      <c r="B123" t="s">
+        <v>138</v>
+      </c>
+      <c r="C123" t="s">
+        <v>139</v>
+      </c>
+      <c r="D123" t="s">
+        <v>44</v>
+      </c>
+      <c r="E123" t="s">
+        <v>45</v>
+      </c>
+      <c r="F123" t="s">
+        <v>43</v>
+      </c>
+      <c r="G123" t="s">
+        <v>43</v>
+      </c>
+      <c r="H123" t="s">
+        <v>43</v>
+      </c>
+      <c r="I123" t="s">
+        <v>43</v>
+      </c>
+      <c r="J123" t="s">
+        <v>43</v>
+      </c>
+      <c r="K123" t="s">
+        <v>46</v>
+      </c>
+      <c r="L123" t="s">
+        <v>140</v>
+      </c>
+      <c r="M123" t="s">
+        <v>141</v>
+      </c>
+      <c r="N123">
+        <v>7</v>
+      </c>
+      <c r="O123">
+        <v>1876</v>
+      </c>
+      <c r="P123">
+        <v>7</v>
+      </c>
+      <c r="Q123">
+        <v>1876</v>
+      </c>
+      <c r="R123" t="s">
+        <v>49</v>
+      </c>
+      <c r="S123" t="s">
+        <v>50</v>
+      </c>
+      <c r="T123" t="s">
+        <v>51</v>
+      </c>
+      <c r="U123" t="s">
+        <v>52</v>
+      </c>
+      <c r="V123" t="s">
+        <v>64</v>
+      </c>
+      <c r="X123" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y123" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA123" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB123">
+        <v>117478</v>
+      </c>
+      <c r="AC123" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD123" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE123" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF123" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG123">
+        <v>9.5238089999999997E-2</v>
+      </c>
+      <c r="AH123" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI123" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ123">
+        <v>21</v>
+      </c>
+      <c r="AK123">
+        <v>1</v>
+      </c>
+      <c r="AL123" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN123" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO123" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>137</v>
+      </c>
+      <c r="B124" t="s">
+        <v>138</v>
+      </c>
+      <c r="C124" t="s">
+        <v>139</v>
+      </c>
+      <c r="D124" t="s">
+        <v>44</v>
+      </c>
+      <c r="E124" t="s">
+        <v>45</v>
+      </c>
+      <c r="F124" t="s">
+        <v>43</v>
+      </c>
+      <c r="G124" t="s">
+        <v>43</v>
+      </c>
+      <c r="H124" t="s">
+        <v>43</v>
+      </c>
+      <c r="I124" t="s">
+        <v>43</v>
+      </c>
+      <c r="J124" t="s">
+        <v>43</v>
+      </c>
+      <c r="K124" t="s">
+        <v>46</v>
+      </c>
+      <c r="L124" t="s">
+        <v>140</v>
+      </c>
+      <c r="M124" t="s">
+        <v>141</v>
+      </c>
+      <c r="N124">
+        <v>7</v>
+      </c>
+      <c r="O124">
+        <v>1876</v>
+      </c>
+      <c r="P124">
+        <v>7</v>
+      </c>
+      <c r="Q124">
+        <v>1876</v>
+      </c>
+      <c r="R124" t="s">
+        <v>49</v>
+      </c>
+      <c r="S124" t="s">
+        <v>50</v>
+      </c>
+      <c r="T124" t="s">
+        <v>51</v>
+      </c>
+      <c r="U124" t="s">
+        <v>52</v>
+      </c>
+      <c r="V124" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA124" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB124">
+        <v>115095</v>
+      </c>
+      <c r="AC124" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE124" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG124">
+        <v>4.7619050000000003E-2</v>
+      </c>
+      <c r="AH124" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI124" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ124">
+        <v>21</v>
+      </c>
+      <c r="AK124">
+        <v>1</v>
+      </c>
+      <c r="AL124" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN124" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO124" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>